<commit_message>
successfully merging two spreadsheets to a new file - now just need to ensure that customers common to both source spreadsheets are detected and not repeated when merging
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -351,7 +351,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,187 @@
       <c r="C16" t="inlineStr">
         <is>
           <t>Ford</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>123</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Marcela</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Wang</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>124</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Andrew</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Wang</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>125</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Roger</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Kondrat</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>126</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Omar</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Hussain</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>127</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Omar</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Wang</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>128</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Bobby</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>129</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Mash</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>It</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>130</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Pop</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Rocks</t>
+        </is>
+      </c>
+    </row>
+    <row r="26"/>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Peter</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Parker</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Stark</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1002</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Bruce</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Banner</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Carol</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Danvers</t>
         </is>
       </c>
     </row>
@@ -570,7 +751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,6 +1291,521 @@
     </row>
     <row r="55"/>
     <row r="56"/>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2222</v>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>43586</v>
+      </c>
+      <c r="C58" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2223</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>43586</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>2224</v>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>43587</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>2225</v>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>43588</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2226</v>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>43588</v>
+      </c>
+      <c r="C62" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2227</v>
+      </c>
+      <c r="B63" s="1" t="n">
+        <v>43590</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>2228</v>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>43590</v>
+      </c>
+      <c r="C64" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2229</v>
+      </c>
+      <c r="B65" s="1" t="n">
+        <v>43590</v>
+      </c>
+      <c r="C65" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2230</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <v>43591</v>
+      </c>
+      <c r="C66" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2231</v>
+      </c>
+      <c r="B67" s="1" t="n">
+        <v>43592</v>
+      </c>
+      <c r="C67" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>2232</v>
+      </c>
+      <c r="B68" s="1" t="n">
+        <v>43592</v>
+      </c>
+      <c r="C68" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2233</v>
+      </c>
+      <c r="B69" s="1" t="n">
+        <v>43593</v>
+      </c>
+      <c r="C69" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2234</v>
+      </c>
+      <c r="B70" s="1" t="n">
+        <v>43594</v>
+      </c>
+      <c r="C70" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>2235</v>
+      </c>
+      <c r="B71" s="1" t="n">
+        <v>43594</v>
+      </c>
+      <c r="C71" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>2236</v>
+      </c>
+      <c r="B72" s="1" t="n">
+        <v>43594</v>
+      </c>
+      <c r="C72" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>2237</v>
+      </c>
+      <c r="B73" s="1" t="n">
+        <v>43595</v>
+      </c>
+      <c r="C73" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>2238</v>
+      </c>
+      <c r="B74" s="1" t="n">
+        <v>43596</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>2239</v>
+      </c>
+      <c r="B75" s="1" t="n">
+        <v>43596</v>
+      </c>
+      <c r="C75" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>2240</v>
+      </c>
+      <c r="B76" s="1" t="n">
+        <v>43597</v>
+      </c>
+      <c r="C76" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>2241</v>
+      </c>
+      <c r="B77" s="1" t="n">
+        <v>43597</v>
+      </c>
+      <c r="C77" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>2242</v>
+      </c>
+      <c r="B78" s="1" t="n">
+        <v>43598</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>2243</v>
+      </c>
+      <c r="B79" s="1" t="n">
+        <v>43599</v>
+      </c>
+      <c r="C79" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>2244</v>
+      </c>
+      <c r="B80" s="1" t="n">
+        <v>43600</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>2245</v>
+      </c>
+      <c r="B81" s="1" t="n">
+        <v>43600</v>
+      </c>
+      <c r="C81" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>2246</v>
+      </c>
+      <c r="B82" s="1" t="n">
+        <v>43601</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>2247</v>
+      </c>
+      <c r="B83" s="1" t="n">
+        <v>43601</v>
+      </c>
+      <c r="C83" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>2248</v>
+      </c>
+      <c r="B84" s="1" t="n">
+        <v>43602</v>
+      </c>
+      <c r="C84" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>2249</v>
+      </c>
+      <c r="B85" s="1" t="n">
+        <v>43603</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>2250</v>
+      </c>
+      <c r="B86" s="1" t="n">
+        <v>43603</v>
+      </c>
+      <c r="C86" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>2251</v>
+      </c>
+      <c r="B87" s="1" t="n">
+        <v>43604</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>2252</v>
+      </c>
+      <c r="B88" s="1" t="n">
+        <v>43604</v>
+      </c>
+      <c r="C88" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>2253</v>
+      </c>
+      <c r="B89" s="1" t="n">
+        <v>43605</v>
+      </c>
+      <c r="C89" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>2254</v>
+      </c>
+      <c r="B90" s="1" t="n">
+        <v>43606</v>
+      </c>
+      <c r="C90" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>2255</v>
+      </c>
+      <c r="B91" s="1" t="n">
+        <v>43607</v>
+      </c>
+      <c r="C91" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>2256</v>
+      </c>
+      <c r="B92" s="1" t="n">
+        <v>43608</v>
+      </c>
+      <c r="C92" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>2257</v>
+      </c>
+      <c r="B93" s="1" t="n">
+        <v>43609</v>
+      </c>
+      <c r="C93" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>2258</v>
+      </c>
+      <c r="B94" s="1" t="n">
+        <v>43610</v>
+      </c>
+      <c r="C94" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>2259</v>
+      </c>
+      <c r="B95" s="1" t="n">
+        <v>43610</v>
+      </c>
+      <c r="C95" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>2260</v>
+      </c>
+      <c r="B96" s="1" t="n">
+        <v>43611</v>
+      </c>
+      <c r="C96" t="n">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>2261</v>
+      </c>
+      <c r="B97" s="1" t="n">
+        <v>43612</v>
+      </c>
+      <c r="C97" t="n">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>2262</v>
+      </c>
+      <c r="B98" s="1" t="n">
+        <v>43612</v>
+      </c>
+      <c r="C98" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>2263</v>
+      </c>
+      <c r="B99" s="1" t="n">
+        <v>43612</v>
+      </c>
+      <c r="C99" t="n">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>2264</v>
+      </c>
+      <c r="B100" s="1" t="n">
+        <v>43613</v>
+      </c>
+      <c r="C100" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>2265</v>
+      </c>
+      <c r="B101" s="1" t="n">
+        <v>43615</v>
+      </c>
+      <c r="C101" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>2266</v>
+      </c>
+      <c r="B102" s="1" t="n">
+        <v>43615</v>
+      </c>
+      <c r="C102" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>2267</v>
+      </c>
+      <c r="B103" s="1" t="n">
+        <v>43615</v>
+      </c>
+      <c r="C103" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1121,7 +1817,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2378,6 +3074,1221 @@
       </c>
       <c r="F81" t="n">
         <v>30</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>1</v>
+      </c>
+      <c r="B83" t="n">
+        <v>2222</v>
+      </c>
+      <c r="C83" t="n">
+        <v>6</v>
+      </c>
+      <c r="D83" t="n">
+        <v>4</v>
+      </c>
+      <c r="F83" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>2</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2222</v>
+      </c>
+      <c r="C84" t="n">
+        <v>3</v>
+      </c>
+      <c r="D84" t="n">
+        <v>8</v>
+      </c>
+      <c r="F84" t="n">
+        <v>560</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Total of all invoices</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>3</v>
+      </c>
+      <c r="B85" t="n">
+        <v>2222</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1</v>
+      </c>
+      <c r="D85" t="n">
+        <v>4</v>
+      </c>
+      <c r="F85" t="n">
+        <v>40</v>
+      </c>
+      <c r="H85" t="n">
+        <v>16350</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>4</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2222</v>
+      </c>
+      <c r="C86" t="n">
+        <v>8</v>
+      </c>
+      <c r="D86" t="n">
+        <v>6</v>
+      </c>
+      <c r="F86" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>5</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2223</v>
+      </c>
+      <c r="C87" t="n">
+        <v>7</v>
+      </c>
+      <c r="D87" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>6</v>
+      </c>
+      <c r="B88" t="n">
+        <v>2223</v>
+      </c>
+      <c r="C88" t="n">
+        <v>3</v>
+      </c>
+      <c r="D88" t="n">
+        <v>6</v>
+      </c>
+      <c r="F88" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>7</v>
+      </c>
+      <c r="B89" t="n">
+        <v>2223</v>
+      </c>
+      <c r="C89" t="n">
+        <v>4</v>
+      </c>
+      <c r="D89" t="n">
+        <v>7</v>
+      </c>
+      <c r="F89" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>8</v>
+      </c>
+      <c r="B90" t="n">
+        <v>2223</v>
+      </c>
+      <c r="C90" t="n">
+        <v>2</v>
+      </c>
+      <c r="D90" t="n">
+        <v>3</v>
+      </c>
+      <c r="F90" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>9</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2224</v>
+      </c>
+      <c r="C91" t="n">
+        <v>5</v>
+      </c>
+      <c r="D91" t="n">
+        <v>6</v>
+      </c>
+      <c r="F91" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>10</v>
+      </c>
+      <c r="B92" t="n">
+        <v>2224</v>
+      </c>
+      <c r="C92" t="n">
+        <v>5</v>
+      </c>
+      <c r="D92" t="n">
+        <v>9</v>
+      </c>
+      <c r="F92" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>11</v>
+      </c>
+      <c r="B93" t="n">
+        <v>2225</v>
+      </c>
+      <c r="C93" t="n">
+        <v>4</v>
+      </c>
+      <c r="D93" t="n">
+        <v>7</v>
+      </c>
+      <c r="F93" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>12</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2225</v>
+      </c>
+      <c r="C94" t="n">
+        <v>2</v>
+      </c>
+      <c r="D94" t="n">
+        <v>5</v>
+      </c>
+      <c r="F94" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>13</v>
+      </c>
+      <c r="B95" t="n">
+        <v>2226</v>
+      </c>
+      <c r="C95" t="n">
+        <v>2</v>
+      </c>
+      <c r="D95" t="n">
+        <v>11</v>
+      </c>
+      <c r="F95" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>14</v>
+      </c>
+      <c r="B96" t="n">
+        <v>2226</v>
+      </c>
+      <c r="C96" t="n">
+        <v>4</v>
+      </c>
+      <c r="D96" t="n">
+        <v>8</v>
+      </c>
+      <c r="F96" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>15</v>
+      </c>
+      <c r="B97" t="n">
+        <v>2227</v>
+      </c>
+      <c r="C97" t="n">
+        <v>4</v>
+      </c>
+      <c r="D97" t="n">
+        <v>9</v>
+      </c>
+      <c r="F97" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>16</v>
+      </c>
+      <c r="B98" t="n">
+        <v>2228</v>
+      </c>
+      <c r="C98" t="n">
+        <v>6</v>
+      </c>
+      <c r="D98" t="n">
+        <v>8</v>
+      </c>
+      <c r="F98" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>17</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2228</v>
+      </c>
+      <c r="C99" t="n">
+        <v>7</v>
+      </c>
+      <c r="D99" t="n">
+        <v>7</v>
+      </c>
+      <c r="F99" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>18</v>
+      </c>
+      <c r="B100" t="n">
+        <v>2229</v>
+      </c>
+      <c r="C100" t="n">
+        <v>6</v>
+      </c>
+      <c r="D100" t="n">
+        <v>9</v>
+      </c>
+      <c r="F100" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>19</v>
+      </c>
+      <c r="B101" t="n">
+        <v>2229</v>
+      </c>
+      <c r="C101" t="n">
+        <v>3</v>
+      </c>
+      <c r="D101" t="n">
+        <v>4</v>
+      </c>
+      <c r="F101" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>20</v>
+      </c>
+      <c r="B102" t="n">
+        <v>2229</v>
+      </c>
+      <c r="C102" t="n">
+        <v>7</v>
+      </c>
+      <c r="D102" t="n">
+        <v>2</v>
+      </c>
+      <c r="F102" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>21</v>
+      </c>
+      <c r="B103" t="n">
+        <v>2230</v>
+      </c>
+      <c r="C103" t="n">
+        <v>3</v>
+      </c>
+      <c r="D103" t="n">
+        <v>9</v>
+      </c>
+      <c r="F103" t="n">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>22</v>
+      </c>
+      <c r="B104" t="n">
+        <v>2230</v>
+      </c>
+      <c r="C104" t="n">
+        <v>3</v>
+      </c>
+      <c r="D104" t="n">
+        <v>5</v>
+      </c>
+      <c r="F104" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>23</v>
+      </c>
+      <c r="B105" t="n">
+        <v>2231</v>
+      </c>
+      <c r="C105" t="n">
+        <v>8</v>
+      </c>
+      <c r="D105" t="n">
+        <v>2</v>
+      </c>
+      <c r="F105" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>24</v>
+      </c>
+      <c r="B106" t="n">
+        <v>2232</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1</v>
+      </c>
+      <c r="D106" t="n">
+        <v>14</v>
+      </c>
+      <c r="F106" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>25</v>
+      </c>
+      <c r="B107" t="n">
+        <v>2233</v>
+      </c>
+      <c r="C107" t="n">
+        <v>4</v>
+      </c>
+      <c r="D107" t="n">
+        <v>4</v>
+      </c>
+      <c r="F107" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>26</v>
+      </c>
+      <c r="B108" t="n">
+        <v>2234</v>
+      </c>
+      <c r="C108" t="n">
+        <v>5</v>
+      </c>
+      <c r="D108" t="n">
+        <v>9</v>
+      </c>
+      <c r="F108" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>27</v>
+      </c>
+      <c r="B109" t="n">
+        <v>2235</v>
+      </c>
+      <c r="C109" t="n">
+        <v>4</v>
+      </c>
+      <c r="D109" t="n">
+        <v>2</v>
+      </c>
+      <c r="F109" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>28</v>
+      </c>
+      <c r="B110" t="n">
+        <v>2236</v>
+      </c>
+      <c r="C110" t="n">
+        <v>4</v>
+      </c>
+      <c r="D110" t="n">
+        <v>9</v>
+      </c>
+      <c r="F110" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>29</v>
+      </c>
+      <c r="B111" t="n">
+        <v>2236</v>
+      </c>
+      <c r="C111" t="n">
+        <v>3</v>
+      </c>
+      <c r="D111" t="n">
+        <v>3</v>
+      </c>
+      <c r="F111" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>30</v>
+      </c>
+      <c r="B112" t="n">
+        <v>2237</v>
+      </c>
+      <c r="C112" t="n">
+        <v>7</v>
+      </c>
+      <c r="D112" t="n">
+        <v>10</v>
+      </c>
+      <c r="F112" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>31</v>
+      </c>
+      <c r="B113" t="n">
+        <v>2238</v>
+      </c>
+      <c r="C113" t="n">
+        <v>8</v>
+      </c>
+      <c r="D113" t="n">
+        <v>12</v>
+      </c>
+      <c r="F113" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>32</v>
+      </c>
+      <c r="B114" t="n">
+        <v>2238</v>
+      </c>
+      <c r="C114" t="n">
+        <v>4</v>
+      </c>
+      <c r="D114" t="n">
+        <v>3</v>
+      </c>
+      <c r="F114" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>33</v>
+      </c>
+      <c r="B115" t="n">
+        <v>2239</v>
+      </c>
+      <c r="C115" t="n">
+        <v>6</v>
+      </c>
+      <c r="D115" t="n">
+        <v>7</v>
+      </c>
+      <c r="F115" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>34</v>
+      </c>
+      <c r="B116" t="n">
+        <v>2239</v>
+      </c>
+      <c r="C116" t="n">
+        <v>1</v>
+      </c>
+      <c r="D116" t="n">
+        <v>10</v>
+      </c>
+      <c r="F116" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>35</v>
+      </c>
+      <c r="B117" t="n">
+        <v>2239</v>
+      </c>
+      <c r="C117" t="n">
+        <v>3</v>
+      </c>
+      <c r="D117" t="n">
+        <v>7</v>
+      </c>
+      <c r="F117" t="n">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>36</v>
+      </c>
+      <c r="B118" t="n">
+        <v>2240</v>
+      </c>
+      <c r="C118" t="n">
+        <v>4</v>
+      </c>
+      <c r="D118" t="n">
+        <v>7</v>
+      </c>
+      <c r="F118" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>37</v>
+      </c>
+      <c r="B119" t="n">
+        <v>2241</v>
+      </c>
+      <c r="C119" t="n">
+        <v>1</v>
+      </c>
+      <c r="D119" t="n">
+        <v>4</v>
+      </c>
+      <c r="F119" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>38</v>
+      </c>
+      <c r="B120" t="n">
+        <v>2242</v>
+      </c>
+      <c r="C120" t="n">
+        <v>4</v>
+      </c>
+      <c r="D120" t="n">
+        <v>9</v>
+      </c>
+      <c r="F120" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>39</v>
+      </c>
+      <c r="B121" t="n">
+        <v>2243</v>
+      </c>
+      <c r="C121" t="n">
+        <v>6</v>
+      </c>
+      <c r="D121" t="n">
+        <v>1</v>
+      </c>
+      <c r="F121" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>40</v>
+      </c>
+      <c r="B122" t="n">
+        <v>2244</v>
+      </c>
+      <c r="C122" t="n">
+        <v>2</v>
+      </c>
+      <c r="D122" t="n">
+        <v>6</v>
+      </c>
+      <c r="F122" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>41</v>
+      </c>
+      <c r="B123" t="n">
+        <v>2244</v>
+      </c>
+      <c r="C123" t="n">
+        <v>5</v>
+      </c>
+      <c r="D123" t="n">
+        <v>8</v>
+      </c>
+      <c r="F123" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>42</v>
+      </c>
+      <c r="B124" t="n">
+        <v>2245</v>
+      </c>
+      <c r="C124" t="n">
+        <v>2</v>
+      </c>
+      <c r="D124" t="n">
+        <v>10</v>
+      </c>
+      <c r="F124" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>43</v>
+      </c>
+      <c r="B125" t="n">
+        <v>2245</v>
+      </c>
+      <c r="C125" t="n">
+        <v>3</v>
+      </c>
+      <c r="D125" t="n">
+        <v>4</v>
+      </c>
+      <c r="F125" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>44</v>
+      </c>
+      <c r="B126" t="n">
+        <v>2246</v>
+      </c>
+      <c r="C126" t="n">
+        <v>2</v>
+      </c>
+      <c r="D126" t="n">
+        <v>8</v>
+      </c>
+      <c r="F126" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>45</v>
+      </c>
+      <c r="B127" t="n">
+        <v>2247</v>
+      </c>
+      <c r="C127" t="n">
+        <v>2</v>
+      </c>
+      <c r="D127" t="n">
+        <v>9</v>
+      </c>
+      <c r="F127" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>46</v>
+      </c>
+      <c r="B128" t="n">
+        <v>2248</v>
+      </c>
+      <c r="C128" t="n">
+        <v>4</v>
+      </c>
+      <c r="D128" t="n">
+        <v>6</v>
+      </c>
+      <c r="F128" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>47</v>
+      </c>
+      <c r="B129" t="n">
+        <v>2249</v>
+      </c>
+      <c r="C129" t="n">
+        <v>6</v>
+      </c>
+      <c r="D129" t="n">
+        <v>8</v>
+      </c>
+      <c r="F129" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>48</v>
+      </c>
+      <c r="B130" t="n">
+        <v>2250</v>
+      </c>
+      <c r="C130" t="n">
+        <v>5</v>
+      </c>
+      <c r="D130" t="n">
+        <v>7</v>
+      </c>
+      <c r="F130" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>49</v>
+      </c>
+      <c r="B131" t="n">
+        <v>2251</v>
+      </c>
+      <c r="C131" t="n">
+        <v>1</v>
+      </c>
+      <c r="D131" t="n">
+        <v>2</v>
+      </c>
+      <c r="F131" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>50</v>
+      </c>
+      <c r="B132" t="n">
+        <v>2252</v>
+      </c>
+      <c r="C132" t="n">
+        <v>4</v>
+      </c>
+      <c r="D132" t="n">
+        <v>9</v>
+      </c>
+      <c r="F132" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>51</v>
+      </c>
+      <c r="B133" t="n">
+        <v>2253</v>
+      </c>
+      <c r="C133" t="n">
+        <v>3</v>
+      </c>
+      <c r="D133" t="n">
+        <v>2</v>
+      </c>
+      <c r="F133" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>52</v>
+      </c>
+      <c r="B134" t="n">
+        <v>2254</v>
+      </c>
+      <c r="C134" t="n">
+        <v>6</v>
+      </c>
+      <c r="D134" t="n">
+        <v>6</v>
+      </c>
+      <c r="F134" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>53</v>
+      </c>
+      <c r="B135" t="n">
+        <v>2255</v>
+      </c>
+      <c r="C135" t="n">
+        <v>3</v>
+      </c>
+      <c r="D135" t="n">
+        <v>2</v>
+      </c>
+      <c r="F135" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>54</v>
+      </c>
+      <c r="B136" t="n">
+        <v>2256</v>
+      </c>
+      <c r="C136" t="n">
+        <v>2</v>
+      </c>
+      <c r="D136" t="n">
+        <v>5</v>
+      </c>
+      <c r="F136" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>55</v>
+      </c>
+      <c r="B137" t="n">
+        <v>2257</v>
+      </c>
+      <c r="C137" t="n">
+        <v>6</v>
+      </c>
+      <c r="D137" t="n">
+        <v>8</v>
+      </c>
+      <c r="F137" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>56</v>
+      </c>
+      <c r="B138" t="n">
+        <v>2258</v>
+      </c>
+      <c r="C138" t="n">
+        <v>4</v>
+      </c>
+      <c r="D138" t="n">
+        <v>2</v>
+      </c>
+      <c r="F138" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>57</v>
+      </c>
+      <c r="B139" t="n">
+        <v>2259</v>
+      </c>
+      <c r="C139" t="n">
+        <v>6</v>
+      </c>
+      <c r="D139" t="n">
+        <v>5</v>
+      </c>
+      <c r="F139" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>58</v>
+      </c>
+      <c r="B140" t="n">
+        <v>2260</v>
+      </c>
+      <c r="C140" t="n">
+        <v>1</v>
+      </c>
+      <c r="D140" t="n">
+        <v>8</v>
+      </c>
+      <c r="F140" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>59</v>
+      </c>
+      <c r="B141" t="n">
+        <v>2261</v>
+      </c>
+      <c r="C141" t="n">
+        <v>2</v>
+      </c>
+      <c r="D141" t="n">
+        <v>3</v>
+      </c>
+      <c r="F141" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>60</v>
+      </c>
+      <c r="B142" t="n">
+        <v>2262</v>
+      </c>
+      <c r="C142" t="n">
+        <v>8</v>
+      </c>
+      <c r="D142" t="n">
+        <v>1</v>
+      </c>
+      <c r="F142" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>61</v>
+      </c>
+      <c r="B143" t="n">
+        <v>2263</v>
+      </c>
+      <c r="C143" t="n">
+        <v>4</v>
+      </c>
+      <c r="D143" t="n">
+        <v>2</v>
+      </c>
+      <c r="F143" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>62</v>
+      </c>
+      <c r="B144" t="n">
+        <v>2264</v>
+      </c>
+      <c r="C144" t="n">
+        <v>2</v>
+      </c>
+      <c r="D144" t="n">
+        <v>3</v>
+      </c>
+      <c r="F144" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>63</v>
+      </c>
+      <c r="B145" t="n">
+        <v>2265</v>
+      </c>
+      <c r="C145" t="n">
+        <v>1</v>
+      </c>
+      <c r="D145" t="n">
+        <v>5</v>
+      </c>
+      <c r="F145" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>64</v>
+      </c>
+      <c r="B146" t="n">
+        <v>2266</v>
+      </c>
+      <c r="C146" t="n">
+        <v>2</v>
+      </c>
+      <c r="D146" t="n">
+        <v>2</v>
+      </c>
+      <c r="F146" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>65</v>
+      </c>
+      <c r="B147" t="n">
+        <v>2266</v>
+      </c>
+      <c r="C147" t="n">
+        <v>1</v>
+      </c>
+      <c r="D147" t="n">
+        <v>8</v>
+      </c>
+      <c r="F147" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>66</v>
+      </c>
+      <c r="B148" t="n">
+        <v>2266</v>
+      </c>
+      <c r="C148" t="n">
+        <v>2</v>
+      </c>
+      <c r="D148" t="n">
+        <v>8</v>
+      </c>
+      <c r="F148" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>67</v>
+      </c>
+      <c r="B149" t="n">
+        <v>2267</v>
+      </c>
+      <c r="C149" t="n">
+        <v>6</v>
+      </c>
+      <c r="D149" t="n">
+        <v>9</v>
+      </c>
+      <c r="F149" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>68</v>
+      </c>
+      <c r="B150" t="n">
+        <v>2267</v>
+      </c>
+      <c r="C150" t="n">
+        <v>7</v>
+      </c>
+      <c r="D150" t="n">
+        <v>3</v>
+      </c>
+      <c r="F150" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>69</v>
+      </c>
+      <c r="B151" t="n">
+        <v>2267</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1</v>
+      </c>
+      <c r="D151" t="n">
+        <v>4</v>
+      </c>
+      <c r="F151" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>70</v>
+      </c>
+      <c r="B152" t="n">
+        <v>2267</v>
+      </c>
+      <c r="C152" t="n">
+        <v>6</v>
+      </c>
+      <c r="D152" t="n">
+        <v>5</v>
+      </c>
+      <c r="F152" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>71</v>
+      </c>
+      <c r="B153" t="n">
+        <v>2267</v>
+      </c>
+      <c r="C153" t="n">
+        <v>3</v>
+      </c>
+      <c r="D153" t="n">
+        <v>3</v>
+      </c>
+      <c r="F153" t="n">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2391,7 +4302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2549,6 +4460,134 @@
         <v>20</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Pencil</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ruler</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Pen</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>70</v>
+      </c>
+      <c r="D13" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Stapler</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>40</v>
+      </c>
+      <c r="D14" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Binder</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Pencil-case</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>7</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Calculator</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>8</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Eraser</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" t="n">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
merging is a complete success: customers common to both source spreadsheets only show once in the merged target. next step: try to remove blank rows...
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -406,7 +406,6 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
     <row r="5">
       <c r="A5" t="n">
         <v>125</v>
@@ -437,7 +436,6 @@
         </is>
       </c>
     </row>
-    <row r="7"/>
     <row r="8">
       <c r="A8" t="n">
         <v>127</v>
@@ -498,7 +496,6 @@
         </is>
       </c>
     </row>
-    <row r="12"/>
     <row r="13">
       <c r="A13" t="n">
         <v>131</v>
@@ -556,126 +553,6 @@
       <c r="C16" t="inlineStr">
         <is>
           <t>Ford</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>123</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Marcela</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Wang</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>124</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Wang</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>125</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Roger</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Kondrat</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>126</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Omar</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Hussain</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>127</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Omar</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Wang</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>128</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Bobby</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Ford</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>129</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Mash</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>It</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>130</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Pop</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Rocks</t>
         </is>
       </c>
     </row>
@@ -751,7 +628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -996,8 +873,6 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22"/>
-    <row r="23"/>
     <row r="24">
       <c r="A24" t="n">
         <v>242</v>
@@ -1097,7 +972,6 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33"/>
     <row r="34">
       <c r="A34" t="n">
         <v>251</v>
@@ -1186,9 +1060,6 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
     <row r="45">
       <c r="A45" t="n">
         <v>259</v>
@@ -1255,7 +1126,6 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51"/>
     <row r="52">
       <c r="A52" t="n">
         <v>265</v>
@@ -1289,58 +1159,78 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55"/>
-    <row r="56"/>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2222</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>43586</v>
+      </c>
+      <c r="C56" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2223</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>43586</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1002</v>
+      </c>
+    </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2222</v>
+        <v>2224</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>43586</v>
+        <v>43587</v>
       </c>
       <c r="C58" t="n">
-        <v>125</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2223</v>
+        <v>2225</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>43586</v>
+        <v>43588</v>
       </c>
       <c r="C59" t="n">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2224</v>
+        <v>2226</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>43587</v>
+        <v>43588</v>
       </c>
       <c r="C60" t="n">
-        <v>1000</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2225</v>
+        <v>2227</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>43588</v>
+        <v>43590</v>
       </c>
       <c r="C61" t="n">
-        <v>1000</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2226</v>
+        <v>2228</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>43588</v>
+        <v>43590</v>
       </c>
       <c r="C62" t="n">
         <v>128</v>
@@ -1348,98 +1238,98 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2227</v>
+        <v>2229</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>43590</v>
       </c>
       <c r="C63" t="n">
-        <v>1002</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2228</v>
+        <v>2230</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>43590</v>
+        <v>43591</v>
       </c>
       <c r="C64" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2229</v>
+        <v>2231</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>43590</v>
+        <v>43592</v>
       </c>
       <c r="C65" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2230</v>
+        <v>2232</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>43591</v>
+        <v>43592</v>
       </c>
       <c r="C66" t="n">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2231</v>
+        <v>2233</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>43592</v>
+        <v>43593</v>
       </c>
       <c r="C67" t="n">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2232</v>
+        <v>2234</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>43592</v>
+        <v>43594</v>
       </c>
       <c r="C68" t="n">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2233</v>
+        <v>2235</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>43593</v>
+        <v>43594</v>
       </c>
       <c r="C69" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2234</v>
+        <v>2236</v>
       </c>
       <c r="B70" s="1" t="n">
         <v>43594</v>
       </c>
       <c r="C70" t="n">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2235</v>
+        <v>2237</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>43594</v>
+        <v>43595</v>
       </c>
       <c r="C71" t="n">
         <v>127</v>
@@ -1447,98 +1337,98 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2236</v>
+        <v>2238</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>43594</v>
+        <v>43596</v>
       </c>
       <c r="C72" t="n">
-        <v>124</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2237</v>
+        <v>2239</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>43595</v>
+        <v>43596</v>
       </c>
       <c r="C73" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2238</v>
+        <v>2240</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>43596</v>
+        <v>43597</v>
       </c>
       <c r="C74" t="n">
-        <v>1001</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2239</v>
+        <v>2241</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>43596</v>
+        <v>43597</v>
       </c>
       <c r="C75" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2240</v>
+        <v>2242</v>
       </c>
       <c r="B76" s="1" t="n">
-        <v>43597</v>
+        <v>43598</v>
       </c>
       <c r="C76" t="n">
-        <v>125</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2241</v>
+        <v>2243</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>43597</v>
+        <v>43599</v>
       </c>
       <c r="C77" t="n">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2242</v>
+        <v>2244</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>43598</v>
+        <v>43600</v>
       </c>
       <c r="C78" t="n">
-        <v>1000</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2243</v>
+        <v>2245</v>
       </c>
       <c r="B79" s="1" t="n">
-        <v>43599</v>
+        <v>43600</v>
       </c>
       <c r="C79" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2244</v>
+        <v>2246</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>43600</v>
+        <v>43601</v>
       </c>
       <c r="C80" t="n">
         <v>1003</v>
@@ -1546,54 +1436,54 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2245</v>
+        <v>2247</v>
       </c>
       <c r="B81" s="1" t="n">
-        <v>43600</v>
+        <v>43601</v>
       </c>
       <c r="C81" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>2246</v>
+        <v>2248</v>
       </c>
       <c r="B82" s="1" t="n">
-        <v>43601</v>
+        <v>43602</v>
       </c>
       <c r="C82" t="n">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>2247</v>
+        <v>2249</v>
       </c>
       <c r="B83" s="1" t="n">
-        <v>43601</v>
+        <v>43603</v>
       </c>
       <c r="C83" t="n">
-        <v>130</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2248</v>
+        <v>2250</v>
       </c>
       <c r="B84" s="1" t="n">
-        <v>43602</v>
+        <v>43603</v>
       </c>
       <c r="C84" t="n">
-        <v>1000</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2249</v>
+        <v>2251</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>43603</v>
+        <v>43604</v>
       </c>
       <c r="C85" t="n">
         <v>1001</v>
@@ -1601,164 +1491,164 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2250</v>
+        <v>2252</v>
       </c>
       <c r="B86" s="1" t="n">
-        <v>43603</v>
+        <v>43604</v>
       </c>
       <c r="C86" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2251</v>
+        <v>2253</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>43604</v>
+        <v>43605</v>
       </c>
       <c r="C87" t="n">
-        <v>1001</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2252</v>
+        <v>2254</v>
       </c>
       <c r="B88" s="1" t="n">
-        <v>43604</v>
+        <v>43606</v>
       </c>
       <c r="C88" t="n">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>2253</v>
+        <v>2255</v>
       </c>
       <c r="B89" s="1" t="n">
-        <v>43605</v>
+        <v>43607</v>
       </c>
       <c r="C89" t="n">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>2254</v>
+        <v>2256</v>
       </c>
       <c r="B90" s="1" t="n">
-        <v>43606</v>
+        <v>43608</v>
       </c>
       <c r="C90" t="n">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>2255</v>
+        <v>2257</v>
       </c>
       <c r="B91" s="1" t="n">
-        <v>43607</v>
+        <v>43609</v>
       </c>
       <c r="C91" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2256</v>
+        <v>2258</v>
       </c>
       <c r="B92" s="1" t="n">
-        <v>43608</v>
+        <v>43610</v>
       </c>
       <c r="C92" t="n">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>2257</v>
+        <v>2259</v>
       </c>
       <c r="B93" s="1" t="n">
-        <v>43609</v>
+        <v>43610</v>
       </c>
       <c r="C93" t="n">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>2258</v>
+        <v>2260</v>
       </c>
       <c r="B94" s="1" t="n">
-        <v>43610</v>
+        <v>43611</v>
       </c>
       <c r="C94" t="n">
-        <v>126</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2259</v>
+        <v>2261</v>
       </c>
       <c r="B95" s="1" t="n">
-        <v>43610</v>
+        <v>43612</v>
       </c>
       <c r="C95" t="n">
-        <v>123</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>2260</v>
+        <v>2262</v>
       </c>
       <c r="B96" s="1" t="n">
-        <v>43611</v>
+        <v>43612</v>
       </c>
       <c r="C96" t="n">
-        <v>1003</v>
+        <v>123</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>2261</v>
+        <v>2263</v>
       </c>
       <c r="B97" s="1" t="n">
         <v>43612</v>
       </c>
       <c r="C97" t="n">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>2262</v>
+        <v>2264</v>
       </c>
       <c r="B98" s="1" t="n">
-        <v>43612</v>
+        <v>43613</v>
       </c>
       <c r="C98" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>2263</v>
+        <v>2265</v>
       </c>
       <c r="B99" s="1" t="n">
-        <v>43612</v>
+        <v>43615</v>
       </c>
       <c r="C99" t="n">
-        <v>1002</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>2264</v>
+        <v>2266</v>
       </c>
       <c r="B100" s="1" t="n">
-        <v>43613</v>
+        <v>43615</v>
       </c>
       <c r="C100" t="n">
         <v>124</v>
@@ -1766,46 +1656,15 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>2265</v>
+        <v>2267</v>
       </c>
       <c r="B101" s="1" t="n">
         <v>43615</v>
       </c>
       <c r="C101" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>2266</v>
-      </c>
-      <c r="B102" s="1" t="n">
-        <v>43615</v>
-      </c>
-      <c r="C102" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>2267</v>
-      </c>
-      <c r="B103" s="1" t="n">
-        <v>43615</v>
-      </c>
-      <c r="C103" t="n">
         <v>125</v>
       </c>
     </row>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1911,7 +1770,6 @@
         <v>15020</v>
       </c>
     </row>
-    <row r="5"/>
     <row r="6">
       <c r="A6" t="n">
         <v>4</v>
@@ -1980,7 +1838,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10"/>
     <row r="11">
       <c r="A11" t="n">
         <v>8</v>
@@ -2168,7 +2025,6 @@
         <v>400</v>
       </c>
     </row>
-    <row r="22"/>
     <row r="23">
       <c r="A23" t="n">
         <v>19</v>
@@ -2305,8 +2161,6 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31"/>
-    <row r="32"/>
     <row r="33">
       <c r="A33" t="n">
         <v>27</v>
@@ -2562,9 +2416,6 @@
         <v>500</v>
       </c>
     </row>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
     <row r="51">
       <c r="A51" t="n">
         <v>42</v>
@@ -2956,7 +2807,6 @@
         <v>630</v>
       </c>
     </row>
-    <row r="74"/>
     <row r="75">
       <c r="A75" t="n">
         <v>65</v>
@@ -4302,7 +4152,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4460,134 +4310,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Pencil</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>10</v>
-      </c>
-      <c r="D11" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Ruler</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Pen</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>70</v>
-      </c>
-      <c r="D13" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>4</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Stapler</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>40</v>
-      </c>
-      <c r="D14" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>5</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Binder</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>10</v>
-      </c>
-      <c r="D15" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>6</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Pencil-case</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>50</v>
-      </c>
-      <c r="D16" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>7</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Calculator</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>100</v>
-      </c>
-      <c r="D17" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>8</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Eraser</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>10</v>
-      </c>
-      <c r="D18" t="n">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
switched to pandas and dataframes in order to remove empty rows, making progress
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -406,6 +406,7 @@
         </is>
       </c>
     </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" t="n">
         <v>125</v>
@@ -436,6 +437,7 @@
         </is>
       </c>
     </row>
+    <row r="7"/>
     <row r="8">
       <c r="A8" t="n">
         <v>127</v>
@@ -496,6 +498,7 @@
         </is>
       </c>
     </row>
+    <row r="12"/>
     <row r="13">
       <c r="A13" t="n">
         <v>131</v>
@@ -556,6 +559,15 @@
         </is>
       </c>
     </row>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
     <row r="26"/>
     <row r="27">
       <c r="A27" t="n">
@@ -628,7 +640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -873,6 +885,8 @@
         <v>127</v>
       </c>
     </row>
+    <row r="22"/>
+    <row r="23"/>
     <row r="24">
       <c r="A24" t="n">
         <v>242</v>
@@ -972,6 +986,7 @@
         <v>126</v>
       </c>
     </row>
+    <row r="33"/>
     <row r="34">
       <c r="A34" t="n">
         <v>251</v>
@@ -1060,6 +1075,9 @@
         <v>126</v>
       </c>
     </row>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
     <row r="45">
       <c r="A45" t="n">
         <v>259</v>
@@ -1126,6 +1144,7 @@
         <v>124</v>
       </c>
     </row>
+    <row r="51"/>
     <row r="52">
       <c r="A52" t="n">
         <v>265</v>
@@ -1159,78 +1178,58 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>2222</v>
-      </c>
-      <c r="B56" s="1" t="n">
-        <v>43586</v>
-      </c>
-      <c r="C56" t="n">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>2223</v>
-      </c>
-      <c r="B57" s="1" t="n">
-        <v>43586</v>
-      </c>
-      <c r="C57" t="n">
-        <v>1002</v>
-      </c>
-    </row>
+    <row r="55"/>
+    <row r="56"/>
     <row r="58">
       <c r="A58" t="n">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>43587</v>
+        <v>43586</v>
       </c>
       <c r="C58" t="n">
-        <v>1000</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2225</v>
+        <v>2223</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>43588</v>
+        <v>43586</v>
       </c>
       <c r="C59" t="n">
-        <v>1000</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>43588</v>
+        <v>43587</v>
       </c>
       <c r="C60" t="n">
-        <v>128</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2227</v>
+        <v>2225</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>43590</v>
+        <v>43588</v>
       </c>
       <c r="C61" t="n">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>43590</v>
+        <v>43588</v>
       </c>
       <c r="C62" t="n">
         <v>128</v>
@@ -1238,98 +1237,98 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2229</v>
+        <v>2227</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>43590</v>
       </c>
       <c r="C63" t="n">
-        <v>127</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2230</v>
+        <v>2228</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>43591</v>
+        <v>43590</v>
       </c>
       <c r="C64" t="n">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2231</v>
+        <v>2229</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>43592</v>
+        <v>43590</v>
       </c>
       <c r="C65" t="n">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2232</v>
+        <v>2230</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>43592</v>
+        <v>43591</v>
       </c>
       <c r="C66" t="n">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2233</v>
+        <v>2231</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>43593</v>
+        <v>43592</v>
       </c>
       <c r="C67" t="n">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2234</v>
+        <v>2232</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>43594</v>
+        <v>43592</v>
       </c>
       <c r="C68" t="n">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2235</v>
+        <v>2233</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>43594</v>
+        <v>43593</v>
       </c>
       <c r="C69" t="n">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2236</v>
+        <v>2234</v>
       </c>
       <c r="B70" s="1" t="n">
         <v>43594</v>
       </c>
       <c r="C70" t="n">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2237</v>
+        <v>2235</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>43595</v>
+        <v>43594</v>
       </c>
       <c r="C71" t="n">
         <v>127</v>
@@ -1337,98 +1336,98 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2238</v>
+        <v>2236</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>43596</v>
+        <v>43594</v>
       </c>
       <c r="C72" t="n">
-        <v>1001</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2239</v>
+        <v>2237</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>43596</v>
+        <v>43595</v>
       </c>
       <c r="C73" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2240</v>
+        <v>2238</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>43597</v>
+        <v>43596</v>
       </c>
       <c r="C74" t="n">
-        <v>125</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2241</v>
+        <v>2239</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>43597</v>
+        <v>43596</v>
       </c>
       <c r="C75" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2242</v>
+        <v>2240</v>
       </c>
       <c r="B76" s="1" t="n">
-        <v>43598</v>
+        <v>43597</v>
       </c>
       <c r="C76" t="n">
-        <v>1000</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2243</v>
+        <v>2241</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>43599</v>
+        <v>43597</v>
       </c>
       <c r="C77" t="n">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2244</v>
+        <v>2242</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>43600</v>
+        <v>43598</v>
       </c>
       <c r="C78" t="n">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2245</v>
+        <v>2243</v>
       </c>
       <c r="B79" s="1" t="n">
-        <v>43600</v>
+        <v>43599</v>
       </c>
       <c r="C79" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2246</v>
+        <v>2244</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>43601</v>
+        <v>43600</v>
       </c>
       <c r="C80" t="n">
         <v>1003</v>
@@ -1436,54 +1435,54 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2247</v>
+        <v>2245</v>
       </c>
       <c r="B81" s="1" t="n">
-        <v>43601</v>
+        <v>43600</v>
       </c>
       <c r="C81" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>2248</v>
+        <v>2246</v>
       </c>
       <c r="B82" s="1" t="n">
-        <v>43602</v>
+        <v>43601</v>
       </c>
       <c r="C82" t="n">
-        <v>1000</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>2249</v>
+        <v>2247</v>
       </c>
       <c r="B83" s="1" t="n">
-        <v>43603</v>
+        <v>43601</v>
       </c>
       <c r="C83" t="n">
-        <v>1001</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2250</v>
+        <v>2248</v>
       </c>
       <c r="B84" s="1" t="n">
-        <v>43603</v>
+        <v>43602</v>
       </c>
       <c r="C84" t="n">
-        <v>126</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2251</v>
+        <v>2249</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>43604</v>
+        <v>43603</v>
       </c>
       <c r="C85" t="n">
         <v>1001</v>
@@ -1491,164 +1490,164 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2252</v>
+        <v>2250</v>
       </c>
       <c r="B86" s="1" t="n">
-        <v>43604</v>
+        <v>43603</v>
       </c>
       <c r="C86" t="n">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2253</v>
+        <v>2251</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>43605</v>
+        <v>43604</v>
       </c>
       <c r="C87" t="n">
-        <v>125</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2254</v>
+        <v>2252</v>
       </c>
       <c r="B88" s="1" t="n">
-        <v>43606</v>
+        <v>43604</v>
       </c>
       <c r="C88" t="n">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>2255</v>
+        <v>2253</v>
       </c>
       <c r="B89" s="1" t="n">
-        <v>43607</v>
+        <v>43605</v>
       </c>
       <c r="C89" t="n">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="B90" s="1" t="n">
-        <v>43608</v>
+        <v>43606</v>
       </c>
       <c r="C90" t="n">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>2257</v>
+        <v>2255</v>
       </c>
       <c r="B91" s="1" t="n">
-        <v>43609</v>
+        <v>43607</v>
       </c>
       <c r="C91" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2258</v>
+        <v>2256</v>
       </c>
       <c r="B92" s="1" t="n">
-        <v>43610</v>
+        <v>43608</v>
       </c>
       <c r="C92" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>2259</v>
+        <v>2257</v>
       </c>
       <c r="B93" s="1" t="n">
-        <v>43610</v>
+        <v>43609</v>
       </c>
       <c r="C93" t="n">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="B94" s="1" t="n">
-        <v>43611</v>
+        <v>43610</v>
       </c>
       <c r="C94" t="n">
-        <v>1003</v>
+        <v>126</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2261</v>
+        <v>2259</v>
       </c>
       <c r="B95" s="1" t="n">
-        <v>43612</v>
+        <v>43610</v>
       </c>
       <c r="C95" t="n">
-        <v>1001</v>
+        <v>123</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>2262</v>
+        <v>2260</v>
       </c>
       <c r="B96" s="1" t="n">
-        <v>43612</v>
+        <v>43611</v>
       </c>
       <c r="C96" t="n">
-        <v>123</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="B97" s="1" t="n">
         <v>43612</v>
       </c>
       <c r="C97" t="n">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>2264</v>
+        <v>2262</v>
       </c>
       <c r="B98" s="1" t="n">
-        <v>43613</v>
+        <v>43612</v>
       </c>
       <c r="C98" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>2265</v>
+        <v>2263</v>
       </c>
       <c r="B99" s="1" t="n">
-        <v>43615</v>
+        <v>43612</v>
       </c>
       <c r="C99" t="n">
-        <v>126</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>2266</v>
+        <v>2264</v>
       </c>
       <c r="B100" s="1" t="n">
-        <v>43615</v>
+        <v>43613</v>
       </c>
       <c r="C100" t="n">
         <v>124</v>
@@ -1656,15 +1655,46 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>2267</v>
+        <v>2265</v>
       </c>
       <c r="B101" s="1" t="n">
         <v>43615</v>
       </c>
       <c r="C101" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>2266</v>
+      </c>
+      <c r="B102" s="1" t="n">
+        <v>43615</v>
+      </c>
+      <c r="C102" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>2267</v>
+      </c>
+      <c r="B103" s="1" t="n">
+        <v>43615</v>
+      </c>
+      <c r="C103" t="n">
         <v>125</v>
       </c>
     </row>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1770,6 +1800,7 @@
         <v>15020</v>
       </c>
     </row>
+    <row r="5"/>
     <row r="6">
       <c r="A6" t="n">
         <v>4</v>
@@ -1838,6 +1869,7 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10"/>
     <row r="11">
       <c r="A11" t="n">
         <v>8</v>
@@ -2025,6 +2057,7 @@
         <v>400</v>
       </c>
     </row>
+    <row r="22"/>
     <row r="23">
       <c r="A23" t="n">
         <v>19</v>
@@ -2161,6 +2194,8 @@
         <v>60</v>
       </c>
     </row>
+    <row r="31"/>
+    <row r="32"/>
     <row r="33">
       <c r="A33" t="n">
         <v>27</v>
@@ -2416,6 +2451,9 @@
         <v>500</v>
       </c>
     </row>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
     <row r="51">
       <c r="A51" t="n">
         <v>42</v>
@@ -2807,6 +2845,7 @@
         <v>630</v>
       </c>
     </row>
+    <row r="74"/>
     <row r="75">
       <c r="A75" t="n">
         <v>65</v>

</xml_diff>

<commit_message>
making progress: successfully wrote sorted dataframe to worksheet, effectively 'removing' blank rows (since they get sorted to the bottom)
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -406,25 +406,39 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>125</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Roger</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Kondrat</t>
+        </is>
+      </c>
+    </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Roger</t>
+          <t>Omar</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Kondrat</t>
+          <t>Hussain</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -433,200 +447,238 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hussain</t>
-        </is>
-      </c>
-    </row>
-    <row r="7"/>
+          <t>Wang</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>128</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Bobby</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+    </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Omar</t>
+          <t>Mash</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Wang</t>
+          <t>It</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bobby</t>
+          <t>Pop</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Rocks</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mash</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>It</t>
+          <t>Sugar</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Pop</t>
+          <t>Pip</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Rocks</t>
-        </is>
-      </c>
-    </row>
-    <row r="12"/>
+          <t>Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>133</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Roman</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Winger</t>
+        </is>
+      </c>
+    </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Bobby</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Sugar</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>132</v>
+        <v>1000</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Pip</t>
+          <t>Peter</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Parker</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>133</v>
+        <v>1001</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Tony</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Winger</t>
+          <t>Stark</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>134</v>
+        <v>1002</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Bobby</t>
+          <t>Bruce</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Ford</t>
-        </is>
-      </c>
-    </row>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
+          <t>Banner</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Carol</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Danvers</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v/>
+      </c>
+    </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Peter</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Parker</t>
-        </is>
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Tony</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Stark</t>
-        </is>
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1002</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Bruce</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Banner</t>
-        </is>
+        <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1003</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Carol</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Danvers</t>
-        </is>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
used dropna() to actually remove dataframe rows that contain NaN in a key column
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -351,7 +351,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,71 +614,6 @@
         <is>
           <t>Danvers</t>
         </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spreadsheet is now 'clean' - all worksheets are sorted by ID, with blank rows removed
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -627,7 +627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -872,36 +872,56 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22"/>
-    <row r="23"/>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>242</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>43568</v>
+      </c>
+      <c r="C22" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>243</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>43569</v>
+      </c>
+      <c r="C23" t="n">
+        <v>130</v>
+      </c>
+    </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>43568</v>
+        <v>43570</v>
       </c>
       <c r="C24" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>43569</v>
+        <v>43570</v>
       </c>
       <c r="C25" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>43570</v>
+        <v>43571</v>
       </c>
       <c r="C26" t="n">
         <v>134</v>
@@ -909,54 +929,54 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>43570</v>
+        <v>43571</v>
       </c>
       <c r="C27" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>43571</v>
+        <v>43572</v>
       </c>
       <c r="C28" t="n">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>43571</v>
+        <v>43573</v>
       </c>
       <c r="C29" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>43572</v>
+        <v>43573</v>
       </c>
       <c r="C30" t="n">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>43573</v>
+        <v>43574</v>
       </c>
       <c r="C31" t="n">
         <v>132</v>
@@ -964,33 +984,43 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>43573</v>
+        <v>43574</v>
       </c>
       <c r="C32" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>253</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>43575</v>
+      </c>
+      <c r="C33" t="n">
+        <v>125</v>
+      </c>
+    </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>43574</v>
+        <v>43576</v>
       </c>
       <c r="C34" t="n">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>43574</v>
+        <v>43577</v>
       </c>
       <c r="C35" t="n">
         <v>128</v>
@@ -998,500 +1028,571 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>43575</v>
+        <v>43578</v>
       </c>
       <c r="C36" t="n">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>43576</v>
+        <v>43579</v>
       </c>
       <c r="C37" t="n">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>43577</v>
+        <v>43580</v>
       </c>
       <c r="C38" t="n">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>43578</v>
+        <v>43580</v>
       </c>
       <c r="C39" t="n">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>43579</v>
+        <v>43581</v>
       </c>
       <c r="C40" t="n">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>43580</v>
+        <v>43582</v>
       </c>
       <c r="C41" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>262</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>43582</v>
+      </c>
+      <c r="C42" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>263</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>43582</v>
+      </c>
+      <c r="C43" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>264</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>43583</v>
+      </c>
+      <c r="C44" t="n">
+        <v>124</v>
+      </c>
+    </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>43580</v>
+        <v>43585</v>
       </c>
       <c r="C45" t="n">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>43581</v>
+        <v>43585</v>
       </c>
       <c r="C46" t="n">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>43582</v>
+        <v>43585</v>
       </c>
       <c r="C47" t="n">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>262</v>
+        <v>2222</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>43582</v>
+        <v>43586</v>
       </c>
       <c r="C48" t="n">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>263</v>
+        <v>2223</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>43582</v>
+        <v>43586</v>
       </c>
       <c r="C49" t="n">
-        <v>133</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>264</v>
+        <v>2224</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>43583</v>
+        <v>43587</v>
       </c>
       <c r="C50" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2225</v>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>43588</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1000</v>
+      </c>
+    </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>265</v>
+        <v>2226</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>43585</v>
+        <v>43588</v>
       </c>
       <c r="C52" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>266</v>
+        <v>2227</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>43585</v>
+        <v>43590</v>
       </c>
       <c r="C53" t="n">
-        <v>124</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>267</v>
+        <v>2228</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>43585</v>
+        <v>43590</v>
       </c>
       <c r="C54" t="n">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55"/>
-    <row r="56"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2229</v>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>43590</v>
+      </c>
+      <c r="C55" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2230</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>43591</v>
+      </c>
+      <c r="C56" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2231</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>43592</v>
+      </c>
+      <c r="C57" t="n">
+        <v>129</v>
+      </c>
+    </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2222</v>
+        <v>2232</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>43586</v>
+        <v>43592</v>
       </c>
       <c r="C58" t="n">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2223</v>
+        <v>2233</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>43586</v>
+        <v>43593</v>
       </c>
       <c r="C59" t="n">
-        <v>1002</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2224</v>
+        <v>2234</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>43587</v>
+        <v>43594</v>
       </c>
       <c r="C60" t="n">
-        <v>1000</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2225</v>
+        <v>2235</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>43588</v>
+        <v>43594</v>
       </c>
       <c r="C61" t="n">
-        <v>1000</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2226</v>
+        <v>2236</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>43588</v>
+        <v>43594</v>
       </c>
       <c r="C62" t="n">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2227</v>
+        <v>2237</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>43590</v>
+        <v>43595</v>
       </c>
       <c r="C63" t="n">
-        <v>1002</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2228</v>
+        <v>2238</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>43590</v>
+        <v>43596</v>
       </c>
       <c r="C64" t="n">
-        <v>128</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2229</v>
+        <v>2239</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>43590</v>
+        <v>43596</v>
       </c>
       <c r="C65" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2230</v>
+        <v>2240</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>43591</v>
+        <v>43597</v>
       </c>
       <c r="C66" t="n">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2231</v>
+        <v>2241</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>43592</v>
+        <v>43597</v>
       </c>
       <c r="C67" t="n">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2232</v>
+        <v>2242</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>43592</v>
+        <v>43598</v>
       </c>
       <c r="C68" t="n">
-        <v>123</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2233</v>
+        <v>2243</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>43593</v>
+        <v>43599</v>
       </c>
       <c r="C69" t="n">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2234</v>
+        <v>2244</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>43594</v>
+        <v>43600</v>
       </c>
       <c r="C70" t="n">
-        <v>130</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2235</v>
+        <v>2245</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>43594</v>
+        <v>43600</v>
       </c>
       <c r="C71" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2236</v>
+        <v>2246</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>43594</v>
+        <v>43601</v>
       </c>
       <c r="C72" t="n">
-        <v>124</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2237</v>
+        <v>2247</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>43595</v>
+        <v>43601</v>
       </c>
       <c r="C73" t="n">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2238</v>
+        <v>2248</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>43596</v>
+        <v>43602</v>
       </c>
       <c r="C74" t="n">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2239</v>
+        <v>2249</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>43596</v>
+        <v>43603</v>
       </c>
       <c r="C75" t="n">
-        <v>126</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2240</v>
+        <v>2250</v>
       </c>
       <c r="B76" s="1" t="n">
-        <v>43597</v>
+        <v>43603</v>
       </c>
       <c r="C76" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2241</v>
+        <v>2251</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>43597</v>
+        <v>43604</v>
       </c>
       <c r="C77" t="n">
-        <v>127</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2242</v>
+        <v>2252</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>43598</v>
+        <v>43604</v>
       </c>
       <c r="C78" t="n">
-        <v>1000</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2243</v>
+        <v>2253</v>
       </c>
       <c r="B79" s="1" t="n">
-        <v>43599</v>
+        <v>43605</v>
       </c>
       <c r="C79" t="n">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2244</v>
+        <v>2254</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>43600</v>
+        <v>43606</v>
       </c>
       <c r="C80" t="n">
-        <v>1003</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2245</v>
+        <v>2255</v>
       </c>
       <c r="B81" s="1" t="n">
-        <v>43600</v>
+        <v>43607</v>
       </c>
       <c r="C81" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>2246</v>
+        <v>2256</v>
       </c>
       <c r="B82" s="1" t="n">
-        <v>43601</v>
+        <v>43608</v>
       </c>
       <c r="C82" t="n">
-        <v>1003</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>2247</v>
+        <v>2257</v>
       </c>
       <c r="B83" s="1" t="n">
-        <v>43601</v>
+        <v>43609</v>
       </c>
       <c r="C83" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2248</v>
+        <v>2258</v>
       </c>
       <c r="B84" s="1" t="n">
-        <v>43602</v>
+        <v>43610</v>
       </c>
       <c r="C84" t="n">
-        <v>1000</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2249</v>
+        <v>2259</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>43603</v>
+        <v>43610</v>
       </c>
       <c r="C85" t="n">
-        <v>1001</v>
+        <v>123</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2250</v>
+        <v>2260</v>
       </c>
       <c r="B86" s="1" t="n">
-        <v>43603</v>
+        <v>43611</v>
       </c>
       <c r="C86" t="n">
-        <v>126</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2251</v>
+        <v>2261</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>43604</v>
+        <v>43612</v>
       </c>
       <c r="C87" t="n">
         <v>1001</v>
@@ -1499,189 +1600,70 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2252</v>
+        <v>2262</v>
       </c>
       <c r="B88" s="1" t="n">
-        <v>43604</v>
+        <v>43612</v>
       </c>
       <c r="C88" t="n">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>2253</v>
+        <v>2263</v>
       </c>
       <c r="B89" s="1" t="n">
-        <v>43605</v>
+        <v>43612</v>
       </c>
       <c r="C89" t="n">
-        <v>125</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>2254</v>
+        <v>2264</v>
       </c>
       <c r="B90" s="1" t="n">
-        <v>43606</v>
+        <v>43613</v>
       </c>
       <c r="C90" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>2255</v>
+        <v>2265</v>
       </c>
       <c r="B91" s="1" t="n">
-        <v>43607</v>
+        <v>43615</v>
       </c>
       <c r="C91" t="n">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2256</v>
+        <v>2266</v>
       </c>
       <c r="B92" s="1" t="n">
-        <v>43608</v>
+        <v>43615</v>
       </c>
       <c r="C92" t="n">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>2257</v>
+        <v>2267</v>
       </c>
       <c r="B93" s="1" t="n">
-        <v>43609</v>
+        <v>43615</v>
       </c>
       <c r="C93" t="n">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>2258</v>
-      </c>
-      <c r="B94" s="1" t="n">
-        <v>43610</v>
-      </c>
-      <c r="C94" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>2259</v>
-      </c>
-      <c r="B95" s="1" t="n">
-        <v>43610</v>
-      </c>
-      <c r="C95" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>2260</v>
-      </c>
-      <c r="B96" s="1" t="n">
-        <v>43611</v>
-      </c>
-      <c r="C96" t="n">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>2261</v>
-      </c>
-      <c r="B97" s="1" t="n">
-        <v>43612</v>
-      </c>
-      <c r="C97" t="n">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>2262</v>
-      </c>
-      <c r="B98" s="1" t="n">
-        <v>43612</v>
-      </c>
-      <c r="C98" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>2263</v>
-      </c>
-      <c r="B99" s="1" t="n">
-        <v>43612</v>
-      </c>
-      <c r="C99" t="n">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>2264</v>
-      </c>
-      <c r="B100" s="1" t="n">
-        <v>43613</v>
-      </c>
-      <c r="C100" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>2265</v>
-      </c>
-      <c r="B101" s="1" t="n">
-        <v>43615</v>
-      </c>
-      <c r="C101" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>2266</v>
-      </c>
-      <c r="B102" s="1" t="n">
-        <v>43615</v>
-      </c>
-      <c r="C102" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>2267</v>
-      </c>
-      <c r="B103" s="1" t="n">
-        <v>43615</v>
-      </c>
-      <c r="C103" t="n">
         <v>125</v>
       </c>
     </row>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1693,7 +1675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H153"/>
+  <dimension ref="A1:H143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1787,445 +1769,525 @@
         <v>15020</v>
       </c>
     </row>
-    <row r="5"/>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>222</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>240</v>
+      </c>
+    </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
-        <v>240</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
         <v>223</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
-        <v>50</v>
+        <v>560</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
         <v>223</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>560</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
         <v>223</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>224</v>
+      </c>
+      <c r="C10" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" t="n">
+        <v>700</v>
+      </c>
+    </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>700</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>50</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
-        <v>210</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C17" t="n">
+        <v>6</v>
+      </c>
+      <c r="D17" t="n">
         <v>5</v>
       </c>
-      <c r="D17" t="n">
-        <v>6</v>
-      </c>
       <c r="F17" t="n">
-        <v>60</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
-        <v>210</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
-        <v>60</v>
+        <v>400</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
-        <v>250</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" t="n">
         <v>229</v>
       </c>
       <c r="C21" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="22"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>230</v>
+      </c>
+      <c r="C22" t="n">
+        <v>5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>9</v>
+      </c>
+      <c r="F22" t="n">
+        <v>90</v>
+      </c>
+    </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D24" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
-        <v>420</v>
+        <v>900</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C25" t="n">
         <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>100</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C27" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
-        <v>900</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C28" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
-        <v>60</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
-        <v>210</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
         <v>5</v>
       </c>
-      <c r="D30" t="n">
-        <v>6</v>
-      </c>
       <c r="F30" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>237</v>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" t="n">
+        <v>8</v>
+      </c>
+      <c r="F31" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32</v>
+      </c>
+      <c r="B32" t="n">
+        <v>238</v>
+      </c>
+      <c r="C32" t="n">
+        <v>8</v>
+      </c>
+      <c r="D32" t="n">
+        <v>6</v>
+      </c>
+      <c r="F32" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="31"/>
-    <row r="32"/>
     <row r="33">
       <c r="A33" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C33" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D33" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
-        <v>350</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
-        <v>160</v>
+        <v>450</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D35" t="n">
         <v>5</v>
@@ -2236,251 +2298,299 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B36" t="n">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C36" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D36" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>320</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D37" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
-        <v>270</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C38" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C39" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C40" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D40" t="n">
         <v>5</v>
       </c>
       <c r="F40" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C41" t="n">
         <v>6</v>
       </c>
       <c r="D41" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
-        <v>450</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C42" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
-        <v>240</v>
+        <v>500</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D43" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C44" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D44" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F44" t="n">
-        <v>200</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C45" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D45" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
-        <v>150</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C46" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>300</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C47" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D47" t="n">
         <v>5</v>
       </c>
       <c r="F47" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>249</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2</v>
+      </c>
+      <c r="D48" t="n">
+        <v>9</v>
+      </c>
+      <c r="F48" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>250</v>
+      </c>
+      <c r="C49" t="n">
+        <v>6</v>
+      </c>
+      <c r="D49" t="n">
+        <v>6</v>
+      </c>
+      <c r="F49" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>251</v>
+      </c>
+      <c r="C50" t="n">
+        <v>7</v>
+      </c>
+      <c r="D50" t="n">
+        <v>5</v>
+      </c>
+      <c r="F50" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
     <row r="51">
       <c r="A51" t="n">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C51" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D51" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="C52" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D52" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
-        <v>450</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C53" t="n">
         <v>4</v>
@@ -2494,44 +2604,44 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="C54" t="n">
         <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C55" t="n">
         <v>4</v>
       </c>
       <c r="D55" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
-        <v>200</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C56" t="n">
         <v>2</v>
@@ -2545,10 +2655,10 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="C57" t="n">
         <v>6</v>
@@ -2562,78 +2672,78 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C58" t="n">
         <v>7</v>
       </c>
       <c r="D58" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C59" t="n">
         <v>5</v>
       </c>
       <c r="D59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C60" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D60" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
-        <v>70</v>
+        <v>450</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C61" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D61" t="n">
         <v>6</v>
       </c>
       <c r="F61" t="n">
-        <v>240</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C62" t="n">
         <v>1</v>
@@ -2647,115 +2757,115 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="C63" t="n">
         <v>4</v>
       </c>
       <c r="D63" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
-        <v>320</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C64" t="n">
         <v>2</v>
       </c>
       <c r="D64" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C65" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D65" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
-        <v>300</v>
+        <v>630</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C66" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D66" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
-        <v>700</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="C67" t="n">
         <v>5</v>
       </c>
       <c r="D67" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B68" t="n">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C68" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D68" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
-        <v>450</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B69" t="n">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C69" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D69" t="n">
         <v>6</v>
@@ -2766,665 +2876,698 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B70" t="n">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C70" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D70" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B71" t="n">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C71" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D71" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
-        <v>240</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B72" t="n">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C72" t="n">
         <v>2</v>
       </c>
       <c r="D72" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="B73" t="n">
-        <v>266</v>
+        <v>2222</v>
       </c>
       <c r="C73" t="n">
+        <v>6</v>
+      </c>
+      <c r="D73" t="n">
+        <v>4</v>
+      </c>
+      <c r="F73" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>2</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2222</v>
+      </c>
+      <c r="C74" t="n">
         <v>3</v>
       </c>
-      <c r="D73" t="n">
-        <v>9</v>
-      </c>
-      <c r="F73" t="n">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="74"/>
+      <c r="D74" t="n">
+        <v>8</v>
+      </c>
+      <c r="F74" t="n">
+        <v>560</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Total of all invoices</t>
+        </is>
+      </c>
+    </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="B75" t="n">
-        <v>266</v>
+        <v>2222</v>
       </c>
       <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="n">
         <v>4</v>
       </c>
-      <c r="D75" t="n">
-        <v>2</v>
-      </c>
       <c r="F75" t="n">
-        <v>80</v>
+        <v>40</v>
+      </c>
+      <c r="H75" t="n">
+        <v>16350</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="B76" t="n">
-        <v>266</v>
+        <v>2222</v>
       </c>
       <c r="C76" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="B77" t="n">
-        <v>267</v>
+        <v>2223</v>
       </c>
       <c r="C77" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="B78" t="n">
-        <v>267</v>
+        <v>2223</v>
       </c>
       <c r="C78" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
-        <v>60</v>
+        <v>280</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="B79" t="n">
-        <v>267</v>
+        <v>2223</v>
       </c>
       <c r="C79" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D79" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
-        <v>60</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="B80" t="n">
-        <v>267</v>
+        <v>2223</v>
       </c>
       <c r="C80" t="n">
         <v>3</v>
       </c>
       <c r="D80" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
-        <v>140</v>
+        <v>420</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="B81" t="n">
-        <v>267</v>
+        <v>2224</v>
       </c>
       <c r="C81" t="n">
         <v>5</v>
       </c>
       <c r="D81" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
-        <v>30</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>10</v>
+      </c>
+      <c r="B82" t="n">
+        <v>2224</v>
+      </c>
+      <c r="C82" t="n">
+        <v>5</v>
+      </c>
+      <c r="D82" t="n">
+        <v>9</v>
+      </c>
+      <c r="F82" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B83" t="n">
-        <v>2222</v>
+        <v>2225</v>
       </c>
       <c r="C83" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D83" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
-        <v>200</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
+        <v>12</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2225</v>
+      </c>
+      <c r="C84" t="n">
         <v>2</v>
       </c>
-      <c r="B84" t="n">
-        <v>2222</v>
-      </c>
-      <c r="C84" t="n">
-        <v>3</v>
-      </c>
       <c r="D84" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
-        <v>560</v>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Total of all invoices</t>
-        </is>
+        <v>150</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B85" t="n">
-        <v>2222</v>
+        <v>2226</v>
       </c>
       <c r="C85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D85" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F85" t="n">
-        <v>40</v>
-      </c>
-      <c r="H85" t="n">
-        <v>16350</v>
+        <v>330</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
+        <v>14</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2226</v>
+      </c>
+      <c r="C86" t="n">
         <v>4</v>
       </c>
-      <c r="B86" t="n">
-        <v>2222</v>
-      </c>
-      <c r="C86" t="n">
+      <c r="D86" t="n">
         <v>8</v>
       </c>
-      <c r="D86" t="n">
-        <v>6</v>
-      </c>
       <c r="F86" t="n">
-        <v>60</v>
+        <v>320</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B87" t="n">
-        <v>2223</v>
+        <v>2227</v>
       </c>
       <c r="C87" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D87" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F87" t="n">
-        <v>200</v>
+        <v>360</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B88" t="n">
-        <v>2223</v>
+        <v>2228</v>
       </c>
       <c r="C88" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D88" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>420</v>
+        <v>700</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B89" t="n">
-        <v>2223</v>
+        <v>2228</v>
       </c>
       <c r="C89" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D89" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F89" t="n">
-        <v>280</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B90" t="n">
-        <v>2223</v>
+        <v>2229</v>
       </c>
       <c r="C90" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D90" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F90" t="n">
-        <v>90</v>
+        <v>450</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B91" t="n">
-        <v>2224</v>
+        <v>2229</v>
       </c>
       <c r="C91" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D91" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
-        <v>60</v>
+        <v>280</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B92" t="n">
-        <v>2224</v>
+        <v>2229</v>
       </c>
       <c r="C92" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D92" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
-        <v>90</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B93" t="n">
-        <v>2225</v>
+        <v>2230</v>
       </c>
       <c r="C93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D93" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
-        <v>280</v>
+        <v>630</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B94" t="n">
-        <v>2225</v>
+        <v>2230</v>
       </c>
       <c r="C94" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D94" t="n">
         <v>5</v>
       </c>
       <c r="F94" t="n">
-        <v>150</v>
+        <v>350</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B95" t="n">
-        <v>2226</v>
+        <v>2231</v>
       </c>
       <c r="C95" t="n">
+        <v>8</v>
+      </c>
+      <c r="D95" t="n">
         <v>2</v>
       </c>
-      <c r="D95" t="n">
-        <v>11</v>
-      </c>
       <c r="F95" t="n">
-        <v>330</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
+        <v>24</v>
+      </c>
+      <c r="B96" t="n">
+        <v>2232</v>
+      </c>
+      <c r="C96" t="n">
+        <v>1</v>
+      </c>
+      <c r="D96" t="n">
         <v>14</v>
       </c>
-      <c r="B96" t="n">
-        <v>2226</v>
-      </c>
-      <c r="C96" t="n">
-        <v>4</v>
-      </c>
-      <c r="D96" t="n">
-        <v>8</v>
-      </c>
       <c r="F96" t="n">
-        <v>320</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B97" t="n">
-        <v>2227</v>
+        <v>2233</v>
       </c>
       <c r="C97" t="n">
         <v>4</v>
       </c>
       <c r="D97" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
-        <v>360</v>
+        <v>160</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B98" t="n">
-        <v>2228</v>
+        <v>2234</v>
       </c>
       <c r="C98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D98" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
-        <v>400</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B99" t="n">
-        <v>2228</v>
+        <v>2235</v>
       </c>
       <c r="C99" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D99" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
-        <v>700</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B100" t="n">
-        <v>2229</v>
+        <v>2236</v>
       </c>
       <c r="C100" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D100" t="n">
         <v>9</v>
       </c>
       <c r="F100" t="n">
-        <v>450</v>
+        <v>360</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B101" t="n">
-        <v>2229</v>
+        <v>2236</v>
       </c>
       <c r="C101" t="n">
         <v>3</v>
       </c>
       <c r="D101" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F101" t="n">
-        <v>280</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B102" t="n">
-        <v>2229</v>
+        <v>2237</v>
       </c>
       <c r="C102" t="n">
         <v>7</v>
       </c>
       <c r="D102" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F102" t="n">
-        <v>200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B103" t="n">
-        <v>2230</v>
+        <v>2238</v>
       </c>
       <c r="C103" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D103" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F103" t="n">
-        <v>630</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B104" t="n">
-        <v>2230</v>
+        <v>2238</v>
       </c>
       <c r="C104" t="n">
+        <v>4</v>
+      </c>
+      <c r="D104" t="n">
         <v>3</v>
       </c>
-      <c r="D104" t="n">
-        <v>5</v>
-      </c>
       <c r="F104" t="n">
-        <v>350</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B105" t="n">
-        <v>2231</v>
+        <v>2239</v>
       </c>
       <c r="C105" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D105" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F105" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B106" t="n">
-        <v>2232</v>
+        <v>2239</v>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D106" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F106" t="n">
-        <v>140</v>
+        <v>490</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B107" t="n">
-        <v>2233</v>
+        <v>2239</v>
       </c>
       <c r="C107" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D107" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F107" t="n">
-        <v>160</v>
+        <v>350</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B108" t="n">
-        <v>2234</v>
+        <v>2240</v>
       </c>
       <c r="C108" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D108" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F108" t="n">
-        <v>90</v>
+        <v>280</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B109" t="n">
-        <v>2235</v>
+        <v>2241</v>
       </c>
       <c r="C109" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" t="n">
         <v>4</v>
       </c>
-      <c r="D109" t="n">
-        <v>2</v>
-      </c>
       <c r="F109" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B110" t="n">
-        <v>2236</v>
+        <v>2242</v>
       </c>
       <c r="C110" t="n">
         <v>4</v>
@@ -3438,237 +3581,237 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B111" t="n">
-        <v>2236</v>
+        <v>2243</v>
       </c>
       <c r="C111" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D111" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F111" t="n">
-        <v>210</v>
+        <v>50</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B112" t="n">
-        <v>2237</v>
+        <v>2244</v>
       </c>
       <c r="C112" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D112" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F112" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B113" t="n">
-        <v>2238</v>
+        <v>2244</v>
       </c>
       <c r="C113" t="n">
+        <v>5</v>
+      </c>
+      <c r="D113" t="n">
         <v>8</v>
       </c>
-      <c r="D113" t="n">
-        <v>12</v>
-      </c>
       <c r="F113" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B114" t="n">
-        <v>2238</v>
+        <v>2245</v>
       </c>
       <c r="C114" t="n">
+        <v>3</v>
+      </c>
+      <c r="D114" t="n">
         <v>4</v>
       </c>
-      <c r="D114" t="n">
-        <v>3</v>
-      </c>
       <c r="F114" t="n">
-        <v>120</v>
+        <v>280</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B115" t="n">
-        <v>2239</v>
+        <v>2245</v>
       </c>
       <c r="C115" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D115" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F115" t="n">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B116" t="n">
-        <v>2239</v>
+        <v>2246</v>
       </c>
       <c r="C116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D116" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F116" t="n">
-        <v>100</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B117" t="n">
-        <v>2239</v>
+        <v>2247</v>
       </c>
       <c r="C117" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D117" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F117" t="n">
-        <v>490</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B118" t="n">
-        <v>2240</v>
+        <v>2248</v>
       </c>
       <c r="C118" t="n">
         <v>4</v>
       </c>
       <c r="D118" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F118" t="n">
-        <v>280</v>
+        <v>240</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B119" t="n">
-        <v>2241</v>
+        <v>2249</v>
       </c>
       <c r="C119" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D119" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F119" t="n">
-        <v>40</v>
+        <v>400</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B120" t="n">
-        <v>2242</v>
+        <v>2250</v>
       </c>
       <c r="C120" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D120" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F120" t="n">
-        <v>360</v>
+        <v>70</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B121" t="n">
-        <v>2243</v>
+        <v>2251</v>
       </c>
       <c r="C121" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F121" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B122" t="n">
-        <v>2244</v>
+        <v>2252</v>
       </c>
       <c r="C122" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D122" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F122" t="n">
-        <v>180</v>
+        <v>360</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B123" t="n">
-        <v>2244</v>
+        <v>2253</v>
       </c>
       <c r="C123" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D123" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F123" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B124" t="n">
-        <v>2245</v>
+        <v>2254</v>
       </c>
       <c r="C124" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D124" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F124" t="n">
         <v>300</v>
@@ -3676,494 +3819,324 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B125" t="n">
-        <v>2245</v>
+        <v>2255</v>
       </c>
       <c r="C125" t="n">
         <v>3</v>
       </c>
       <c r="D125" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F125" t="n">
-        <v>280</v>
+        <v>140</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B126" t="n">
-        <v>2246</v>
+        <v>2256</v>
       </c>
       <c r="C126" t="n">
         <v>2</v>
       </c>
       <c r="D126" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F126" t="n">
-        <v>240</v>
+        <v>150</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B127" t="n">
-        <v>2247</v>
+        <v>2257</v>
       </c>
       <c r="C127" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D127" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F127" t="n">
-        <v>270</v>
+        <v>400</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B128" t="n">
-        <v>2248</v>
+        <v>2258</v>
       </c>
       <c r="C128" t="n">
         <v>4</v>
       </c>
       <c r="D128" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F128" t="n">
-        <v>240</v>
+        <v>80</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B129" t="n">
-        <v>2249</v>
+        <v>2259</v>
       </c>
       <c r="C129" t="n">
         <v>6</v>
       </c>
       <c r="D129" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F129" t="n">
-        <v>400</v>
+        <v>250</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B130" t="n">
-        <v>2250</v>
+        <v>2260</v>
       </c>
       <c r="C130" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D130" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F130" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B131" t="n">
-        <v>2251</v>
+        <v>2261</v>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D131" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F131" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B132" t="n">
-        <v>2252</v>
+        <v>2262</v>
       </c>
       <c r="C132" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D132" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F132" t="n">
-        <v>360</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B133" t="n">
-        <v>2253</v>
+        <v>2263</v>
       </c>
       <c r="C133" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D133" t="n">
         <v>2</v>
       </c>
       <c r="F133" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B134" t="n">
-        <v>2254</v>
+        <v>2264</v>
       </c>
       <c r="C134" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D134" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F134" t="n">
-        <v>300</v>
+        <v>90</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B135" t="n">
-        <v>2255</v>
+        <v>2265</v>
       </c>
       <c r="C135" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D135" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F135" t="n">
-        <v>140</v>
+        <v>50</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B136" t="n">
-        <v>2256</v>
+        <v>2266</v>
       </c>
       <c r="C136" t="n">
         <v>2</v>
       </c>
       <c r="D136" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F136" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B137" t="n">
-        <v>2257</v>
+        <v>2266</v>
       </c>
       <c r="C137" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D137" t="n">
         <v>8</v>
       </c>
       <c r="F137" t="n">
-        <v>400</v>
+        <v>80</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B138" t="n">
-        <v>2258</v>
+        <v>2266</v>
       </c>
       <c r="C138" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D138" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F138" t="n">
-        <v>80</v>
+        <v>240</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B139" t="n">
-        <v>2259</v>
+        <v>2267</v>
       </c>
       <c r="C139" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D139" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F139" t="n">
-        <v>250</v>
+        <v>40</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B140" t="n">
-        <v>2260</v>
+        <v>2267</v>
       </c>
       <c r="C140" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D140" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F140" t="n">
-        <v>80</v>
+        <v>250</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B141" t="n">
-        <v>2261</v>
+        <v>2267</v>
       </c>
       <c r="C141" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D141" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F141" t="n">
-        <v>90</v>
+        <v>450</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B142" t="n">
-        <v>2262</v>
+        <v>2267</v>
       </c>
       <c r="C142" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D142" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F142" t="n">
-        <v>10</v>
+        <v>300</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B143" t="n">
-        <v>2263</v>
+        <v>2267</v>
       </c>
       <c r="C143" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D143" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F143" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="n">
-        <v>62</v>
-      </c>
-      <c r="B144" t="n">
-        <v>2264</v>
-      </c>
-      <c r="C144" t="n">
-        <v>2</v>
-      </c>
-      <c r="D144" t="n">
-        <v>3</v>
-      </c>
-      <c r="F144" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="n">
-        <v>63</v>
-      </c>
-      <c r="B145" t="n">
-        <v>2265</v>
-      </c>
-      <c r="C145" t="n">
-        <v>1</v>
-      </c>
-      <c r="D145" t="n">
-        <v>5</v>
-      </c>
-      <c r="F145" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="n">
-        <v>64</v>
-      </c>
-      <c r="B146" t="n">
-        <v>2266</v>
-      </c>
-      <c r="C146" t="n">
-        <v>2</v>
-      </c>
-      <c r="D146" t="n">
-        <v>2</v>
-      </c>
-      <c r="F146" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="n">
-        <v>65</v>
-      </c>
-      <c r="B147" t="n">
-        <v>2266</v>
-      </c>
-      <c r="C147" t="n">
-        <v>1</v>
-      </c>
-      <c r="D147" t="n">
-        <v>8</v>
-      </c>
-      <c r="F147" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="n">
-        <v>66</v>
-      </c>
-      <c r="B148" t="n">
-        <v>2266</v>
-      </c>
-      <c r="C148" t="n">
-        <v>2</v>
-      </c>
-      <c r="D148" t="n">
-        <v>8</v>
-      </c>
-      <c r="F148" t="n">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="n">
-        <v>67</v>
-      </c>
-      <c r="B149" t="n">
-        <v>2267</v>
-      </c>
-      <c r="C149" t="n">
-        <v>6</v>
-      </c>
-      <c r="D149" t="n">
-        <v>9</v>
-      </c>
-      <c r="F149" t="n">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="n">
-        <v>68</v>
-      </c>
-      <c r="B150" t="n">
-        <v>2267</v>
-      </c>
-      <c r="C150" t="n">
-        <v>7</v>
-      </c>
-      <c r="D150" t="n">
-        <v>3</v>
-      </c>
-      <c r="F150" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>69</v>
-      </c>
-      <c r="B151" t="n">
-        <v>2267</v>
-      </c>
-      <c r="C151" t="n">
-        <v>1</v>
-      </c>
-      <c r="D151" t="n">
-        <v>4</v>
-      </c>
-      <c r="F151" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="n">
-        <v>70</v>
-      </c>
-      <c r="B152" t="n">
-        <v>2267</v>
-      </c>
-      <c r="C152" t="n">
-        <v>6</v>
-      </c>
-      <c r="D152" t="n">
-        <v>5</v>
-      </c>
-      <c r="F152" t="n">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="n">
-        <v>71</v>
-      </c>
-      <c r="B153" t="n">
-        <v>2267</v>
-      </c>
-      <c r="C153" t="n">
-        <v>3</v>
-      </c>
-      <c r="D153" t="n">
-        <v>3</v>
-      </c>
-      <c r="F153" t="n">
         <v>210</v>
       </c>
     </row>

</xml_diff>

<commit_message>
styling output: made column headers bold
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -22,13 +22,16 @@
   <numFmts count="1">
     <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,8 +54,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -360,21 +364,23 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Customer</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Last</t>
         </is>
       </c>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -636,27 +642,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Invoice</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Customer</t>
         </is>
       </c>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>222</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>43556</v>
       </c>
       <c r="C2" t="n">
@@ -667,7 +675,7 @@
       <c r="A3" t="n">
         <v>223</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>43556</v>
       </c>
       <c r="C3" t="n">
@@ -678,7 +686,7 @@
       <c r="A4" t="n">
         <v>224</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>43557</v>
       </c>
       <c r="C4" t="n">
@@ -689,7 +697,7 @@
       <c r="A5" t="n">
         <v>225</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>43558</v>
       </c>
       <c r="C5" t="n">
@@ -700,7 +708,7 @@
       <c r="A6" t="n">
         <v>226</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>43558</v>
       </c>
       <c r="C6" t="n">
@@ -711,7 +719,7 @@
       <c r="A7" t="n">
         <v>227</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>43559</v>
       </c>
       <c r="C7" t="n">
@@ -722,7 +730,7 @@
       <c r="A8" t="n">
         <v>228</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>43560</v>
       </c>
       <c r="C8" t="n">
@@ -733,7 +741,7 @@
       <c r="A9" t="n">
         <v>229</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>43560</v>
       </c>
       <c r="C9" t="n">
@@ -744,7 +752,7 @@
       <c r="A10" t="n">
         <v>230</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="2" t="n">
         <v>43561</v>
       </c>
       <c r="C10" t="n">
@@ -755,7 +763,7 @@
       <c r="A11" t="n">
         <v>231</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="2" t="n">
         <v>43562</v>
       </c>
       <c r="C11" t="n">
@@ -766,7 +774,7 @@
       <c r="A12" t="n">
         <v>232</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="2" t="n">
         <v>43562</v>
       </c>
       <c r="C12" t="n">
@@ -777,7 +785,7 @@
       <c r="A13" t="n">
         <v>233</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="2" t="n">
         <v>43563</v>
       </c>
       <c r="C13" t="n">
@@ -788,7 +796,7 @@
       <c r="A14" t="n">
         <v>234</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="2" t="n">
         <v>43564</v>
       </c>
       <c r="C14" t="n">
@@ -799,7 +807,7 @@
       <c r="A15" t="n">
         <v>235</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="2" t="n">
         <v>43564</v>
       </c>
       <c r="C15" t="n">
@@ -810,7 +818,7 @@
       <c r="A16" t="n">
         <v>236</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="2" t="n">
         <v>43564</v>
       </c>
       <c r="C16" t="n">
@@ -821,7 +829,7 @@
       <c r="A17" t="n">
         <v>237</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="2" t="n">
         <v>43565</v>
       </c>
       <c r="C17" t="n">
@@ -832,7 +840,7 @@
       <c r="A18" t="n">
         <v>238</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="2" t="n">
         <v>43566</v>
       </c>
       <c r="C18" t="n">
@@ -843,7 +851,7 @@
       <c r="A19" t="n">
         <v>239</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="2" t="n">
         <v>43566</v>
       </c>
       <c r="C19" t="n">
@@ -854,7 +862,7 @@
       <c r="A20" t="n">
         <v>240</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="2" t="n">
         <v>43567</v>
       </c>
       <c r="C20" t="n">
@@ -865,7 +873,7 @@
       <c r="A21" t="n">
         <v>241</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="2" t="n">
         <v>43567</v>
       </c>
       <c r="C21" t="n">
@@ -876,7 +884,7 @@
       <c r="A22" t="n">
         <v>242</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="2" t="n">
         <v>43568</v>
       </c>
       <c r="C22" t="n">
@@ -887,7 +895,7 @@
       <c r="A23" t="n">
         <v>243</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="2" t="n">
         <v>43569</v>
       </c>
       <c r="C23" t="n">
@@ -898,7 +906,7 @@
       <c r="A24" t="n">
         <v>244</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="2" t="n">
         <v>43570</v>
       </c>
       <c r="C24" t="n">
@@ -909,7 +917,7 @@
       <c r="A25" t="n">
         <v>245</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="2" t="n">
         <v>43570</v>
       </c>
       <c r="C25" t="n">
@@ -920,7 +928,7 @@
       <c r="A26" t="n">
         <v>246</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="2" t="n">
         <v>43571</v>
       </c>
       <c r="C26" t="n">
@@ -931,7 +939,7 @@
       <c r="A27" t="n">
         <v>247</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="2" t="n">
         <v>43571</v>
       </c>
       <c r="C27" t="n">
@@ -942,7 +950,7 @@
       <c r="A28" t="n">
         <v>248</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="2" t="n">
         <v>43572</v>
       </c>
       <c r="C28" t="n">
@@ -953,7 +961,7 @@
       <c r="A29" t="n">
         <v>249</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="2" t="n">
         <v>43573</v>
       </c>
       <c r="C29" t="n">
@@ -964,7 +972,7 @@
       <c r="A30" t="n">
         <v>250</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="2" t="n">
         <v>43573</v>
       </c>
       <c r="C30" t="n">
@@ -975,7 +983,7 @@
       <c r="A31" t="n">
         <v>251</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="2" t="n">
         <v>43574</v>
       </c>
       <c r="C31" t="n">
@@ -986,7 +994,7 @@
       <c r="A32" t="n">
         <v>252</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="2" t="n">
         <v>43574</v>
       </c>
       <c r="C32" t="n">
@@ -997,7 +1005,7 @@
       <c r="A33" t="n">
         <v>253</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="2" t="n">
         <v>43575</v>
       </c>
       <c r="C33" t="n">
@@ -1008,7 +1016,7 @@
       <c r="A34" t="n">
         <v>254</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="2" t="n">
         <v>43576</v>
       </c>
       <c r="C34" t="n">
@@ -1019,7 +1027,7 @@
       <c r="A35" t="n">
         <v>255</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="2" t="n">
         <v>43577</v>
       </c>
       <c r="C35" t="n">
@@ -1030,7 +1038,7 @@
       <c r="A36" t="n">
         <v>256</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="2" t="n">
         <v>43578</v>
       </c>
       <c r="C36" t="n">
@@ -1041,7 +1049,7 @@
       <c r="A37" t="n">
         <v>257</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="2" t="n">
         <v>43579</v>
       </c>
       <c r="C37" t="n">
@@ -1052,7 +1060,7 @@
       <c r="A38" t="n">
         <v>258</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="2" t="n">
         <v>43580</v>
       </c>
       <c r="C38" t="n">
@@ -1063,7 +1071,7 @@
       <c r="A39" t="n">
         <v>259</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="2" t="n">
         <v>43580</v>
       </c>
       <c r="C39" t="n">
@@ -1074,7 +1082,7 @@
       <c r="A40" t="n">
         <v>260</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="2" t="n">
         <v>43581</v>
       </c>
       <c r="C40" t="n">
@@ -1085,7 +1093,7 @@
       <c r="A41" t="n">
         <v>261</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="2" t="n">
         <v>43582</v>
       </c>
       <c r="C41" t="n">
@@ -1096,7 +1104,7 @@
       <c r="A42" t="n">
         <v>262</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="2" t="n">
         <v>43582</v>
       </c>
       <c r="C42" t="n">
@@ -1107,7 +1115,7 @@
       <c r="A43" t="n">
         <v>263</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="2" t="n">
         <v>43582</v>
       </c>
       <c r="C43" t="n">
@@ -1118,7 +1126,7 @@
       <c r="A44" t="n">
         <v>264</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="2" t="n">
         <v>43583</v>
       </c>
       <c r="C44" t="n">
@@ -1129,7 +1137,7 @@
       <c r="A45" t="n">
         <v>265</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="2" t="n">
         <v>43585</v>
       </c>
       <c r="C45" t="n">
@@ -1140,7 +1148,7 @@
       <c r="A46" t="n">
         <v>266</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="2" t="n">
         <v>43585</v>
       </c>
       <c r="C46" t="n">
@@ -1151,7 +1159,7 @@
       <c r="A47" t="n">
         <v>267</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="2" t="n">
         <v>43585</v>
       </c>
       <c r="C47" t="n">
@@ -1162,7 +1170,7 @@
       <c r="A48" t="n">
         <v>2222</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="2" t="n">
         <v>43586</v>
       </c>
       <c r="C48" t="n">
@@ -1173,7 +1181,7 @@
       <c r="A49" t="n">
         <v>2223</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="2" t="n">
         <v>43586</v>
       </c>
       <c r="C49" t="n">
@@ -1184,7 +1192,7 @@
       <c r="A50" t="n">
         <v>2224</v>
       </c>
-      <c r="B50" s="1" t="n">
+      <c r="B50" s="2" t="n">
         <v>43587</v>
       </c>
       <c r="C50" t="n">
@@ -1195,7 +1203,7 @@
       <c r="A51" t="n">
         <v>2225</v>
       </c>
-      <c r="B51" s="1" t="n">
+      <c r="B51" s="2" t="n">
         <v>43588</v>
       </c>
       <c r="C51" t="n">
@@ -1206,7 +1214,7 @@
       <c r="A52" t="n">
         <v>2226</v>
       </c>
-      <c r="B52" s="1" t="n">
+      <c r="B52" s="2" t="n">
         <v>43588</v>
       </c>
       <c r="C52" t="n">
@@ -1217,7 +1225,7 @@
       <c r="A53" t="n">
         <v>2227</v>
       </c>
-      <c r="B53" s="1" t="n">
+      <c r="B53" s="2" t="n">
         <v>43590</v>
       </c>
       <c r="C53" t="n">
@@ -1228,7 +1236,7 @@
       <c r="A54" t="n">
         <v>2228</v>
       </c>
-      <c r="B54" s="1" t="n">
+      <c r="B54" s="2" t="n">
         <v>43590</v>
       </c>
       <c r="C54" t="n">
@@ -1239,7 +1247,7 @@
       <c r="A55" t="n">
         <v>2229</v>
       </c>
-      <c r="B55" s="1" t="n">
+      <c r="B55" s="2" t="n">
         <v>43590</v>
       </c>
       <c r="C55" t="n">
@@ -1250,7 +1258,7 @@
       <c r="A56" t="n">
         <v>2230</v>
       </c>
-      <c r="B56" s="1" t="n">
+      <c r="B56" s="2" t="n">
         <v>43591</v>
       </c>
       <c r="C56" t="n">
@@ -1261,7 +1269,7 @@
       <c r="A57" t="n">
         <v>2231</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="2" t="n">
         <v>43592</v>
       </c>
       <c r="C57" t="n">
@@ -1272,7 +1280,7 @@
       <c r="A58" t="n">
         <v>2232</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="2" t="n">
         <v>43592</v>
       </c>
       <c r="C58" t="n">
@@ -1283,7 +1291,7 @@
       <c r="A59" t="n">
         <v>2233</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="B59" s="2" t="n">
         <v>43593</v>
       </c>
       <c r="C59" t="n">
@@ -1294,7 +1302,7 @@
       <c r="A60" t="n">
         <v>2234</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="2" t="n">
         <v>43594</v>
       </c>
       <c r="C60" t="n">
@@ -1305,7 +1313,7 @@
       <c r="A61" t="n">
         <v>2235</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="B61" s="2" t="n">
         <v>43594</v>
       </c>
       <c r="C61" t="n">
@@ -1316,7 +1324,7 @@
       <c r="A62" t="n">
         <v>2236</v>
       </c>
-      <c r="B62" s="1" t="n">
+      <c r="B62" s="2" t="n">
         <v>43594</v>
       </c>
       <c r="C62" t="n">
@@ -1327,7 +1335,7 @@
       <c r="A63" t="n">
         <v>2237</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="2" t="n">
         <v>43595</v>
       </c>
       <c r="C63" t="n">
@@ -1338,7 +1346,7 @@
       <c r="A64" t="n">
         <v>2238</v>
       </c>
-      <c r="B64" s="1" t="n">
+      <c r="B64" s="2" t="n">
         <v>43596</v>
       </c>
       <c r="C64" t="n">
@@ -1349,7 +1357,7 @@
       <c r="A65" t="n">
         <v>2239</v>
       </c>
-      <c r="B65" s="1" t="n">
+      <c r="B65" s="2" t="n">
         <v>43596</v>
       </c>
       <c r="C65" t="n">
@@ -1360,7 +1368,7 @@
       <c r="A66" t="n">
         <v>2240</v>
       </c>
-      <c r="B66" s="1" t="n">
+      <c r="B66" s="2" t="n">
         <v>43597</v>
       </c>
       <c r="C66" t="n">
@@ -1371,7 +1379,7 @@
       <c r="A67" t="n">
         <v>2241</v>
       </c>
-      <c r="B67" s="1" t="n">
+      <c r="B67" s="2" t="n">
         <v>43597</v>
       </c>
       <c r="C67" t="n">
@@ -1382,7 +1390,7 @@
       <c r="A68" t="n">
         <v>2242</v>
       </c>
-      <c r="B68" s="1" t="n">
+      <c r="B68" s="2" t="n">
         <v>43598</v>
       </c>
       <c r="C68" t="n">
@@ -1393,7 +1401,7 @@
       <c r="A69" t="n">
         <v>2243</v>
       </c>
-      <c r="B69" s="1" t="n">
+      <c r="B69" s="2" t="n">
         <v>43599</v>
       </c>
       <c r="C69" t="n">
@@ -1404,7 +1412,7 @@
       <c r="A70" t="n">
         <v>2244</v>
       </c>
-      <c r="B70" s="1" t="n">
+      <c r="B70" s="2" t="n">
         <v>43600</v>
       </c>
       <c r="C70" t="n">
@@ -1415,7 +1423,7 @@
       <c r="A71" t="n">
         <v>2245</v>
       </c>
-      <c r="B71" s="1" t="n">
+      <c r="B71" s="2" t="n">
         <v>43600</v>
       </c>
       <c r="C71" t="n">
@@ -1426,7 +1434,7 @@
       <c r="A72" t="n">
         <v>2246</v>
       </c>
-      <c r="B72" s="1" t="n">
+      <c r="B72" s="2" t="n">
         <v>43601</v>
       </c>
       <c r="C72" t="n">
@@ -1437,7 +1445,7 @@
       <c r="A73" t="n">
         <v>2247</v>
       </c>
-      <c r="B73" s="1" t="n">
+      <c r="B73" s="2" t="n">
         <v>43601</v>
       </c>
       <c r="C73" t="n">
@@ -1448,7 +1456,7 @@
       <c r="A74" t="n">
         <v>2248</v>
       </c>
-      <c r="B74" s="1" t="n">
+      <c r="B74" s="2" t="n">
         <v>43602</v>
       </c>
       <c r="C74" t="n">
@@ -1459,7 +1467,7 @@
       <c r="A75" t="n">
         <v>2249</v>
       </c>
-      <c r="B75" s="1" t="n">
+      <c r="B75" s="2" t="n">
         <v>43603</v>
       </c>
       <c r="C75" t="n">
@@ -1470,7 +1478,7 @@
       <c r="A76" t="n">
         <v>2250</v>
       </c>
-      <c r="B76" s="1" t="n">
+      <c r="B76" s="2" t="n">
         <v>43603</v>
       </c>
       <c r="C76" t="n">
@@ -1481,7 +1489,7 @@
       <c r="A77" t="n">
         <v>2251</v>
       </c>
-      <c r="B77" s="1" t="n">
+      <c r="B77" s="2" t="n">
         <v>43604</v>
       </c>
       <c r="C77" t="n">
@@ -1492,7 +1500,7 @@
       <c r="A78" t="n">
         <v>2252</v>
       </c>
-      <c r="B78" s="1" t="n">
+      <c r="B78" s="2" t="n">
         <v>43604</v>
       </c>
       <c r="C78" t="n">
@@ -1503,7 +1511,7 @@
       <c r="A79" t="n">
         <v>2253</v>
       </c>
-      <c r="B79" s="1" t="n">
+      <c r="B79" s="2" t="n">
         <v>43605</v>
       </c>
       <c r="C79" t="n">
@@ -1514,7 +1522,7 @@
       <c r="A80" t="n">
         <v>2254</v>
       </c>
-      <c r="B80" s="1" t="n">
+      <c r="B80" s="2" t="n">
         <v>43606</v>
       </c>
       <c r="C80" t="n">
@@ -1525,7 +1533,7 @@
       <c r="A81" t="n">
         <v>2255</v>
       </c>
-      <c r="B81" s="1" t="n">
+      <c r="B81" s="2" t="n">
         <v>43607</v>
       </c>
       <c r="C81" t="n">
@@ -1536,7 +1544,7 @@
       <c r="A82" t="n">
         <v>2256</v>
       </c>
-      <c r="B82" s="1" t="n">
+      <c r="B82" s="2" t="n">
         <v>43608</v>
       </c>
       <c r="C82" t="n">
@@ -1547,7 +1555,7 @@
       <c r="A83" t="n">
         <v>2257</v>
       </c>
-      <c r="B83" s="1" t="n">
+      <c r="B83" s="2" t="n">
         <v>43609</v>
       </c>
       <c r="C83" t="n">
@@ -1558,7 +1566,7 @@
       <c r="A84" t="n">
         <v>2258</v>
       </c>
-      <c r="B84" s="1" t="n">
+      <c r="B84" s="2" t="n">
         <v>43610</v>
       </c>
       <c r="C84" t="n">
@@ -1569,7 +1577,7 @@
       <c r="A85" t="n">
         <v>2259</v>
       </c>
-      <c r="B85" s="1" t="n">
+      <c r="B85" s="2" t="n">
         <v>43610</v>
       </c>
       <c r="C85" t="n">
@@ -1580,7 +1588,7 @@
       <c r="A86" t="n">
         <v>2260</v>
       </c>
-      <c r="B86" s="1" t="n">
+      <c r="B86" s="2" t="n">
         <v>43611</v>
       </c>
       <c r="C86" t="n">
@@ -1591,7 +1599,7 @@
       <c r="A87" t="n">
         <v>2261</v>
       </c>
-      <c r="B87" s="1" t="n">
+      <c r="B87" s="2" t="n">
         <v>43612</v>
       </c>
       <c r="C87" t="n">
@@ -1602,7 +1610,7 @@
       <c r="A88" t="n">
         <v>2262</v>
       </c>
-      <c r="B88" s="1" t="n">
+      <c r="B88" s="2" t="n">
         <v>43612</v>
       </c>
       <c r="C88" t="n">
@@ -1613,7 +1621,7 @@
       <c r="A89" t="n">
         <v>2263</v>
       </c>
-      <c r="B89" s="1" t="n">
+      <c r="B89" s="2" t="n">
         <v>43612</v>
       </c>
       <c r="C89" t="n">
@@ -1624,7 +1632,7 @@
       <c r="A90" t="n">
         <v>2264</v>
       </c>
-      <c r="B90" s="1" t="n">
+      <c r="B90" s="2" t="n">
         <v>43613</v>
       </c>
       <c r="C90" t="n">
@@ -1635,7 +1643,7 @@
       <c r="A91" t="n">
         <v>2265</v>
       </c>
-      <c r="B91" s="1" t="n">
+      <c r="B91" s="2" t="n">
         <v>43615</v>
       </c>
       <c r="C91" t="n">
@@ -1646,7 +1654,7 @@
       <c r="A92" t="n">
         <v>2266</v>
       </c>
-      <c r="B92" s="1" t="n">
+      <c r="B92" s="2" t="n">
         <v>43615</v>
       </c>
       <c r="C92" t="n">
@@ -1657,7 +1665,7 @@
       <c r="A93" t="n">
         <v>2267</v>
       </c>
-      <c r="B93" s="1" t="n">
+      <c r="B93" s="2" t="n">
         <v>43615</v>
       </c>
       <c r="C93" t="n">
@@ -1684,31 +1692,34 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Line</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Invoice</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>line total</t>
         </is>
       </c>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -4160,22 +4171,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Price </t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Inventory</t>
         </is>

</xml_diff>

<commit_message>
resolved issue where invoice data was showing as an integer
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -19,8 +19,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD" numFmtId="165"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -57,20 +58,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
     <cellStyle hidden="0" name="basic" xfId="1"/>
     <cellStyle hidden="0" name="basic_bold" xfId="2"/>
+    <cellStyle hidden="0" name="date_style" xfId="3"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -371,9 +375,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.25" defaultRowHeight="25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <sheetData>
-    <row customHeight="1" ht="18" r="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Customer</t>
@@ -392,7 +396,7 @@
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="2">
+    <row r="2">
       <c r="A2" s="2" t="n">
         <v>123</v>
       </c>
@@ -409,7 +413,7 @@
       <c r="D2" s="2" t="n"/>
       <c r="E2" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="3">
+    <row r="3">
       <c r="A3" s="2" t="n">
         <v>124</v>
       </c>
@@ -426,7 +430,7 @@
       <c r="D3" s="2" t="n"/>
       <c r="E3" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="4">
+    <row r="4">
       <c r="A4" s="2" t="n">
         <v>125</v>
       </c>
@@ -443,7 +447,7 @@
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="5">
+    <row r="5">
       <c r="A5" s="2" t="n">
         <v>126</v>
       </c>
@@ -460,7 +464,7 @@
       <c r="D5" s="2" t="n"/>
       <c r="E5" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="6">
+    <row r="6">
       <c r="A6" s="2" t="n">
         <v>127</v>
       </c>
@@ -477,7 +481,7 @@
       <c r="D6" s="2" t="n"/>
       <c r="E6" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="7">
+    <row r="7">
       <c r="A7" s="2" t="n">
         <v>128</v>
       </c>
@@ -494,7 +498,7 @@
       <c r="D7" s="2" t="n"/>
       <c r="E7" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="8">
+    <row r="8">
       <c r="A8" s="2" t="n">
         <v>129</v>
       </c>
@@ -511,7 +515,7 @@
       <c r="D8" s="2" t="n"/>
       <c r="E8" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="9">
+    <row r="9">
       <c r="A9" s="2" t="n">
         <v>130</v>
       </c>
@@ -528,7 +532,7 @@
       <c r="D9" s="2" t="n"/>
       <c r="E9" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="10">
+    <row r="10">
       <c r="A10" s="2" t="n">
         <v>131</v>
       </c>
@@ -545,7 +549,7 @@
       <c r="D10" s="2" t="n"/>
       <c r="E10" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="11">
+    <row r="11">
       <c r="A11" s="2" t="n">
         <v>132</v>
       </c>
@@ -562,7 +566,7 @@
       <c r="D11" s="2" t="n"/>
       <c r="E11" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="12">
+    <row r="12">
       <c r="A12" s="2" t="n">
         <v>133</v>
       </c>
@@ -579,7 +583,7 @@
       <c r="D12" s="2" t="n"/>
       <c r="E12" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="13">
+    <row r="13">
       <c r="A13" s="2" t="n">
         <v>134</v>
       </c>
@@ -596,7 +600,7 @@
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="14">
+    <row r="14">
       <c r="A14" s="2" t="n">
         <v>1000</v>
       </c>
@@ -613,7 +617,7 @@
       <c r="D14" s="2" t="n"/>
       <c r="E14" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="15">
+    <row r="15">
       <c r="A15" s="2" t="n">
         <v>1001</v>
       </c>
@@ -630,7 +634,7 @@
       <c r="D15" s="2" t="n"/>
       <c r="E15" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="16">
+    <row r="16">
       <c r="A16" s="2" t="n">
         <v>1002</v>
       </c>
@@ -647,7 +651,7 @@
       <c r="D16" s="2" t="n"/>
       <c r="E16" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="17">
+    <row r="17">
       <c r="A17" s="2" t="n">
         <v>1003</v>
       </c>
@@ -681,7 +685,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.25" defaultRowHeight="25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -706,7 +710,7 @@
       <c r="A2" s="2" t="n">
         <v>222</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>43556</v>
       </c>
       <c r="C2" s="2" t="n">
@@ -719,7 +723,7 @@
       <c r="A3" s="2" t="n">
         <v>223</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>43556</v>
       </c>
       <c r="C3" s="2" t="n">
@@ -732,7 +736,7 @@
       <c r="A4" s="2" t="n">
         <v>224</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>43557</v>
       </c>
       <c r="C4" s="2" t="n">
@@ -745,7 +749,7 @@
       <c r="A5" s="2" t="n">
         <v>225</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>43558</v>
       </c>
       <c r="C5" s="2" t="n">
@@ -758,7 +762,7 @@
       <c r="A6" s="2" t="n">
         <v>226</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>43558</v>
       </c>
       <c r="C6" s="2" t="n">
@@ -771,7 +775,7 @@
       <c r="A7" s="2" t="n">
         <v>227</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <v>43559</v>
       </c>
       <c r="C7" s="2" t="n">
@@ -784,7 +788,7 @@
       <c r="A8" s="2" t="n">
         <v>228</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="3" t="n">
         <v>43560</v>
       </c>
       <c r="C8" s="2" t="n">
@@ -797,7 +801,7 @@
       <c r="A9" s="2" t="n">
         <v>229</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="3" t="n">
         <v>43560</v>
       </c>
       <c r="C9" s="2" t="n">
@@ -810,7 +814,7 @@
       <c r="A10" s="2" t="n">
         <v>230</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="3" t="n">
         <v>43561</v>
       </c>
       <c r="C10" s="2" t="n">
@@ -823,7 +827,7 @@
       <c r="A11" s="2" t="n">
         <v>231</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="3" t="n">
         <v>43562</v>
       </c>
       <c r="C11" s="2" t="n">
@@ -836,7 +840,7 @@
       <c r="A12" s="2" t="n">
         <v>232</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="3" t="n">
         <v>43562</v>
       </c>
       <c r="C12" s="2" t="n">
@@ -849,7 +853,7 @@
       <c r="A13" s="2" t="n">
         <v>233</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="3" t="n">
         <v>43563</v>
       </c>
       <c r="C13" s="2" t="n">
@@ -862,7 +866,7 @@
       <c r="A14" s="2" t="n">
         <v>234</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="3" t="n">
         <v>43564</v>
       </c>
       <c r="C14" s="2" t="n">
@@ -875,7 +879,7 @@
       <c r="A15" s="2" t="n">
         <v>235</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="3" t="n">
         <v>43564</v>
       </c>
       <c r="C15" s="2" t="n">
@@ -888,7 +892,7 @@
       <c r="A16" s="2" t="n">
         <v>236</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="3" t="n">
         <v>43564</v>
       </c>
       <c r="C16" s="2" t="n">
@@ -901,7 +905,7 @@
       <c r="A17" s="2" t="n">
         <v>237</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="3" t="n">
         <v>43565</v>
       </c>
       <c r="C17" s="2" t="n">
@@ -910,11 +914,11 @@
       <c r="D17" s="2" t="n"/>
       <c r="E17" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="18">
+    <row r="18">
       <c r="A18" s="2" t="n">
         <v>238</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="3" t="n">
         <v>43566</v>
       </c>
       <c r="C18" s="2" t="n">
@@ -923,11 +927,11 @@
       <c r="D18" s="2" t="n"/>
       <c r="E18" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="19">
+    <row r="19">
       <c r="A19" s="2" t="n">
         <v>239</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="3" t="n">
         <v>43566</v>
       </c>
       <c r="C19" s="2" t="n">
@@ -936,11 +940,11 @@
       <c r="D19" s="2" t="n"/>
       <c r="E19" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="20">
+    <row r="20">
       <c r="A20" s="2" t="n">
         <v>240</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="3" t="n">
         <v>43567</v>
       </c>
       <c r="C20" s="2" t="n">
@@ -949,11 +953,11 @@
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="21">
+    <row r="21">
       <c r="A21" s="2" t="n">
         <v>241</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="3" t="n">
         <v>43567</v>
       </c>
       <c r="C21" s="2" t="n">
@@ -962,11 +966,11 @@
       <c r="D21" s="2" t="n"/>
       <c r="E21" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="22">
+    <row r="22">
       <c r="A22" s="2" t="n">
         <v>242</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="3" t="n">
         <v>43568</v>
       </c>
       <c r="C22" s="2" t="n">
@@ -975,11 +979,11 @@
       <c r="D22" s="2" t="n"/>
       <c r="E22" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="23">
+    <row r="23">
       <c r="A23" s="2" t="n">
         <v>243</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="3" t="n">
         <v>43569</v>
       </c>
       <c r="C23" s="2" t="n">
@@ -988,11 +992,11 @@
       <c r="D23" s="2" t="n"/>
       <c r="E23" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="24">
+    <row r="24">
       <c r="A24" s="2" t="n">
         <v>244</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="3" t="n">
         <v>43570</v>
       </c>
       <c r="C24" s="2" t="n">
@@ -1001,11 +1005,11 @@
       <c r="D24" s="2" t="n"/>
       <c r="E24" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="25">
+    <row r="25">
       <c r="A25" s="2" t="n">
         <v>245</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="3" t="n">
         <v>43570</v>
       </c>
       <c r="C25" s="2" t="n">
@@ -1014,11 +1018,11 @@
       <c r="D25" s="2" t="n"/>
       <c r="E25" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="26">
+    <row r="26">
       <c r="A26" s="2" t="n">
         <v>246</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="3" t="n">
         <v>43571</v>
       </c>
       <c r="C26" s="2" t="n">
@@ -1027,11 +1031,11 @@
       <c r="D26" s="2" t="n"/>
       <c r="E26" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="27">
+    <row r="27">
       <c r="A27" s="2" t="n">
         <v>247</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="3" t="n">
         <v>43571</v>
       </c>
       <c r="C27" s="2" t="n">
@@ -1040,11 +1044,11 @@
       <c r="D27" s="2" t="n"/>
       <c r="E27" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="28">
+    <row r="28">
       <c r="A28" s="2" t="n">
         <v>248</v>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="3" t="n">
         <v>43572</v>
       </c>
       <c r="C28" s="2" t="n">
@@ -1053,11 +1057,11 @@
       <c r="D28" s="2" t="n"/>
       <c r="E28" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="29">
+    <row r="29">
       <c r="A29" s="2" t="n">
         <v>249</v>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="3" t="n">
         <v>43573</v>
       </c>
       <c r="C29" s="2" t="n">
@@ -1066,11 +1070,11 @@
       <c r="D29" s="2" t="n"/>
       <c r="E29" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="30">
+    <row r="30">
       <c r="A30" s="2" t="n">
         <v>250</v>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="B30" s="3" t="n">
         <v>43573</v>
       </c>
       <c r="C30" s="2" t="n">
@@ -1079,11 +1083,11 @@
       <c r="D30" s="2" t="n"/>
       <c r="E30" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="31">
+    <row r="31">
       <c r="A31" s="2" t="n">
         <v>251</v>
       </c>
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="3" t="n">
         <v>43574</v>
       </c>
       <c r="C31" s="2" t="n">
@@ -1092,11 +1096,11 @@
       <c r="D31" s="2" t="n"/>
       <c r="E31" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="32">
+    <row r="32">
       <c r="A32" s="2" t="n">
         <v>252</v>
       </c>
-      <c r="B32" s="2" t="n">
+      <c r="B32" s="3" t="n">
         <v>43574</v>
       </c>
       <c r="C32" s="2" t="n">
@@ -1105,11 +1109,11 @@
       <c r="D32" s="2" t="n"/>
       <c r="E32" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="33">
+    <row r="33">
       <c r="A33" s="2" t="n">
         <v>253</v>
       </c>
-      <c r="B33" s="2" t="n">
+      <c r="B33" s="3" t="n">
         <v>43575</v>
       </c>
       <c r="C33" s="2" t="n">
@@ -1118,11 +1122,11 @@
       <c r="D33" s="2" t="n"/>
       <c r="E33" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="34">
+    <row r="34">
       <c r="A34" s="2" t="n">
         <v>254</v>
       </c>
-      <c r="B34" s="2" t="n">
+      <c r="B34" s="3" t="n">
         <v>43576</v>
       </c>
       <c r="C34" s="2" t="n">
@@ -1131,11 +1135,11 @@
       <c r="D34" s="2" t="n"/>
       <c r="E34" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="35">
+    <row r="35">
       <c r="A35" s="2" t="n">
         <v>255</v>
       </c>
-      <c r="B35" s="2" t="n">
+      <c r="B35" s="3" t="n">
         <v>43577</v>
       </c>
       <c r="C35" s="2" t="n">
@@ -1144,11 +1148,11 @@
       <c r="D35" s="2" t="n"/>
       <c r="E35" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="36">
+    <row r="36">
       <c r="A36" s="2" t="n">
         <v>256</v>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="3" t="n">
         <v>43578</v>
       </c>
       <c r="C36" s="2" t="n">
@@ -1157,11 +1161,11 @@
       <c r="D36" s="2" t="n"/>
       <c r="E36" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="37">
+    <row r="37">
       <c r="A37" s="2" t="n">
         <v>257</v>
       </c>
-      <c r="B37" s="2" t="n">
+      <c r="B37" s="3" t="n">
         <v>43579</v>
       </c>
       <c r="C37" s="2" t="n">
@@ -1170,11 +1174,11 @@
       <c r="D37" s="2" t="n"/>
       <c r="E37" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="38">
+    <row r="38">
       <c r="A38" s="2" t="n">
         <v>258</v>
       </c>
-      <c r="B38" s="2" t="n">
+      <c r="B38" s="3" t="n">
         <v>43580</v>
       </c>
       <c r="C38" s="2" t="n">
@@ -1183,11 +1187,11 @@
       <c r="D38" s="2" t="n"/>
       <c r="E38" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="39">
+    <row r="39">
       <c r="A39" s="2" t="n">
         <v>259</v>
       </c>
-      <c r="B39" s="2" t="n">
+      <c r="B39" s="3" t="n">
         <v>43580</v>
       </c>
       <c r="C39" s="2" t="n">
@@ -1196,11 +1200,11 @@
       <c r="D39" s="2" t="n"/>
       <c r="E39" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="40">
+    <row r="40">
       <c r="A40" s="2" t="n">
         <v>260</v>
       </c>
-      <c r="B40" s="2" t="n">
+      <c r="B40" s="3" t="n">
         <v>43581</v>
       </c>
       <c r="C40" s="2" t="n">
@@ -1209,11 +1213,11 @@
       <c r="D40" s="2" t="n"/>
       <c r="E40" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="41">
+    <row r="41">
       <c r="A41" s="2" t="n">
         <v>261</v>
       </c>
-      <c r="B41" s="2" t="n">
+      <c r="B41" s="3" t="n">
         <v>43582</v>
       </c>
       <c r="C41" s="2" t="n">
@@ -1222,11 +1226,11 @@
       <c r="D41" s="2" t="n"/>
       <c r="E41" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="42">
+    <row r="42">
       <c r="A42" s="2" t="n">
         <v>262</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B42" s="3" t="n">
         <v>43582</v>
       </c>
       <c r="C42" s="2" t="n">
@@ -1235,11 +1239,11 @@
       <c r="D42" s="2" t="n"/>
       <c r="E42" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="43">
+    <row r="43">
       <c r="A43" s="2" t="n">
         <v>263</v>
       </c>
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="3" t="n">
         <v>43582</v>
       </c>
       <c r="C43" s="2" t="n">
@@ -1248,11 +1252,11 @@
       <c r="D43" s="2" t="n"/>
       <c r="E43" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="44">
+    <row r="44">
       <c r="A44" s="2" t="n">
         <v>264</v>
       </c>
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="3" t="n">
         <v>43583</v>
       </c>
       <c r="C44" s="2" t="n">
@@ -1261,11 +1265,11 @@
       <c r="D44" s="2" t="n"/>
       <c r="E44" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="45">
+    <row r="45">
       <c r="A45" s="2" t="n">
         <v>265</v>
       </c>
-      <c r="B45" s="2" t="n">
+      <c r="B45" s="3" t="n">
         <v>43585</v>
       </c>
       <c r="C45" s="2" t="n">
@@ -1274,11 +1278,11 @@
       <c r="D45" s="2" t="n"/>
       <c r="E45" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="46">
+    <row r="46">
       <c r="A46" s="2" t="n">
         <v>266</v>
       </c>
-      <c r="B46" s="2" t="n">
+      <c r="B46" s="3" t="n">
         <v>43585</v>
       </c>
       <c r="C46" s="2" t="n">
@@ -1287,11 +1291,11 @@
       <c r="D46" s="2" t="n"/>
       <c r="E46" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="47">
+    <row r="47">
       <c r="A47" s="2" t="n">
         <v>267</v>
       </c>
-      <c r="B47" s="2" t="n">
+      <c r="B47" s="3" t="n">
         <v>43585</v>
       </c>
       <c r="C47" s="2" t="n">
@@ -1300,11 +1304,11 @@
       <c r="D47" s="2" t="n"/>
       <c r="E47" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="48">
+    <row r="48">
       <c r="A48" s="2" t="n">
         <v>2222</v>
       </c>
-      <c r="B48" s="2" t="n">
+      <c r="B48" s="3" t="n">
         <v>43586</v>
       </c>
       <c r="C48" s="2" t="n">
@@ -1313,11 +1317,11 @@
       <c r="D48" s="2" t="n"/>
       <c r="E48" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="49">
+    <row r="49">
       <c r="A49" s="2" t="n">
         <v>2223</v>
       </c>
-      <c r="B49" s="2" t="n">
+      <c r="B49" s="3" t="n">
         <v>43586</v>
       </c>
       <c r="C49" s="2" t="n">
@@ -1326,11 +1330,11 @@
       <c r="D49" s="2" t="n"/>
       <c r="E49" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="50">
+    <row r="50">
       <c r="A50" s="2" t="n">
         <v>2224</v>
       </c>
-      <c r="B50" s="2" t="n">
+      <c r="B50" s="3" t="n">
         <v>43587</v>
       </c>
       <c r="C50" s="2" t="n">
@@ -1339,11 +1343,11 @@
       <c r="D50" s="2" t="n"/>
       <c r="E50" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="51">
+    <row r="51">
       <c r="A51" s="2" t="n">
         <v>2225</v>
       </c>
-      <c r="B51" s="2" t="n">
+      <c r="B51" s="3" t="n">
         <v>43588</v>
       </c>
       <c r="C51" s="2" t="n">
@@ -1352,11 +1356,11 @@
       <c r="D51" s="2" t="n"/>
       <c r="E51" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="52">
+    <row r="52">
       <c r="A52" s="2" t="n">
         <v>2226</v>
       </c>
-      <c r="B52" s="2" t="n">
+      <c r="B52" s="3" t="n">
         <v>43588</v>
       </c>
       <c r="C52" s="2" t="n">
@@ -1365,11 +1369,11 @@
       <c r="D52" s="2" t="n"/>
       <c r="E52" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="53">
+    <row r="53">
       <c r="A53" s="2" t="n">
         <v>2227</v>
       </c>
-      <c r="B53" s="2" t="n">
+      <c r="B53" s="3" t="n">
         <v>43590</v>
       </c>
       <c r="C53" s="2" t="n">
@@ -1378,11 +1382,11 @@
       <c r="D53" s="2" t="n"/>
       <c r="E53" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="54">
+    <row r="54">
       <c r="A54" s="2" t="n">
         <v>2228</v>
       </c>
-      <c r="B54" s="2" t="n">
+      <c r="B54" s="3" t="n">
         <v>43590</v>
       </c>
       <c r="C54" s="2" t="n">
@@ -1391,11 +1395,11 @@
       <c r="D54" s="2" t="n"/>
       <c r="E54" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="55">
+    <row r="55">
       <c r="A55" s="2" t="n">
         <v>2229</v>
       </c>
-      <c r="B55" s="2" t="n">
+      <c r="B55" s="3" t="n">
         <v>43590</v>
       </c>
       <c r="C55" s="2" t="n">
@@ -1404,11 +1408,11 @@
       <c r="D55" s="2" t="n"/>
       <c r="E55" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="56">
+    <row r="56">
       <c r="A56" s="2" t="n">
         <v>2230</v>
       </c>
-      <c r="B56" s="2" t="n">
+      <c r="B56" s="3" t="n">
         <v>43591</v>
       </c>
       <c r="C56" s="2" t="n">
@@ -1417,11 +1421,11 @@
       <c r="D56" s="2" t="n"/>
       <c r="E56" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="57">
+    <row r="57">
       <c r="A57" s="2" t="n">
         <v>2231</v>
       </c>
-      <c r="B57" s="2" t="n">
+      <c r="B57" s="3" t="n">
         <v>43592</v>
       </c>
       <c r="C57" s="2" t="n">
@@ -1430,11 +1434,11 @@
       <c r="D57" s="2" t="n"/>
       <c r="E57" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="58">
+    <row r="58">
       <c r="A58" s="2" t="n">
         <v>2232</v>
       </c>
-      <c r="B58" s="2" t="n">
+      <c r="B58" s="3" t="n">
         <v>43592</v>
       </c>
       <c r="C58" s="2" t="n">
@@ -1443,11 +1447,11 @@
       <c r="D58" s="2" t="n"/>
       <c r="E58" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="59">
+    <row r="59">
       <c r="A59" s="2" t="n">
         <v>2233</v>
       </c>
-      <c r="B59" s="2" t="n">
+      <c r="B59" s="3" t="n">
         <v>43593</v>
       </c>
       <c r="C59" s="2" t="n">
@@ -1456,11 +1460,11 @@
       <c r="D59" s="2" t="n"/>
       <c r="E59" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="60">
+    <row r="60">
       <c r="A60" s="2" t="n">
         <v>2234</v>
       </c>
-      <c r="B60" s="2" t="n">
+      <c r="B60" s="3" t="n">
         <v>43594</v>
       </c>
       <c r="C60" s="2" t="n">
@@ -1469,11 +1473,11 @@
       <c r="D60" s="2" t="n"/>
       <c r="E60" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="61">
+    <row r="61">
       <c r="A61" s="2" t="n">
         <v>2235</v>
       </c>
-      <c r="B61" s="2" t="n">
+      <c r="B61" s="3" t="n">
         <v>43594</v>
       </c>
       <c r="C61" s="2" t="n">
@@ -1482,11 +1486,11 @@
       <c r="D61" s="2" t="n"/>
       <c r="E61" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="62">
+    <row r="62">
       <c r="A62" s="2" t="n">
         <v>2236</v>
       </c>
-      <c r="B62" s="2" t="n">
+      <c r="B62" s="3" t="n">
         <v>43594</v>
       </c>
       <c r="C62" s="2" t="n">
@@ -1495,11 +1499,11 @@
       <c r="D62" s="2" t="n"/>
       <c r="E62" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="63">
+    <row r="63">
       <c r="A63" s="2" t="n">
         <v>2237</v>
       </c>
-      <c r="B63" s="2" t="n">
+      <c r="B63" s="3" t="n">
         <v>43595</v>
       </c>
       <c r="C63" s="2" t="n">
@@ -1508,11 +1512,11 @@
       <c r="D63" s="2" t="n"/>
       <c r="E63" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="64">
+    <row r="64">
       <c r="A64" s="2" t="n">
         <v>2238</v>
       </c>
-      <c r="B64" s="2" t="n">
+      <c r="B64" s="3" t="n">
         <v>43596</v>
       </c>
       <c r="C64" s="2" t="n">
@@ -1521,11 +1525,11 @@
       <c r="D64" s="2" t="n"/>
       <c r="E64" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="65">
+    <row r="65">
       <c r="A65" s="2" t="n">
         <v>2239</v>
       </c>
-      <c r="B65" s="2" t="n">
+      <c r="B65" s="3" t="n">
         <v>43596</v>
       </c>
       <c r="C65" s="2" t="n">
@@ -1534,11 +1538,11 @@
       <c r="D65" s="2" t="n"/>
       <c r="E65" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="66">
+    <row r="66">
       <c r="A66" s="2" t="n">
         <v>2240</v>
       </c>
-      <c r="B66" s="2" t="n">
+      <c r="B66" s="3" t="n">
         <v>43597</v>
       </c>
       <c r="C66" s="2" t="n">
@@ -1547,11 +1551,11 @@
       <c r="D66" s="2" t="n"/>
       <c r="E66" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="67">
+    <row r="67">
       <c r="A67" s="2" t="n">
         <v>2241</v>
       </c>
-      <c r="B67" s="2" t="n">
+      <c r="B67" s="3" t="n">
         <v>43597</v>
       </c>
       <c r="C67" s="2" t="n">
@@ -1560,11 +1564,11 @@
       <c r="D67" s="2" t="n"/>
       <c r="E67" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="68">
+    <row r="68">
       <c r="A68" s="2" t="n">
         <v>2242</v>
       </c>
-      <c r="B68" s="2" t="n">
+      <c r="B68" s="3" t="n">
         <v>43598</v>
       </c>
       <c r="C68" s="2" t="n">
@@ -1573,11 +1577,11 @@
       <c r="D68" s="2" t="n"/>
       <c r="E68" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="69">
+    <row r="69">
       <c r="A69" s="2" t="n">
         <v>2243</v>
       </c>
-      <c r="B69" s="2" t="n">
+      <c r="B69" s="3" t="n">
         <v>43599</v>
       </c>
       <c r="C69" s="2" t="n">
@@ -1586,11 +1590,11 @@
       <c r="D69" s="2" t="n"/>
       <c r="E69" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="70">
+    <row r="70">
       <c r="A70" s="2" t="n">
         <v>2244</v>
       </c>
-      <c r="B70" s="2" t="n">
+      <c r="B70" s="3" t="n">
         <v>43600</v>
       </c>
       <c r="C70" s="2" t="n">
@@ -1599,11 +1603,11 @@
       <c r="D70" s="2" t="n"/>
       <c r="E70" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="71">
+    <row r="71">
       <c r="A71" s="2" t="n">
         <v>2245</v>
       </c>
-      <c r="B71" s="2" t="n">
+      <c r="B71" s="3" t="n">
         <v>43600</v>
       </c>
       <c r="C71" s="2" t="n">
@@ -1612,11 +1616,11 @@
       <c r="D71" s="2" t="n"/>
       <c r="E71" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="72">
+    <row r="72">
       <c r="A72" s="2" t="n">
         <v>2246</v>
       </c>
-      <c r="B72" s="2" t="n">
+      <c r="B72" s="3" t="n">
         <v>43601</v>
       </c>
       <c r="C72" s="2" t="n">
@@ -1625,11 +1629,11 @@
       <c r="D72" s="2" t="n"/>
       <c r="E72" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="73">
+    <row r="73">
       <c r="A73" s="2" t="n">
         <v>2247</v>
       </c>
-      <c r="B73" s="2" t="n">
+      <c r="B73" s="3" t="n">
         <v>43601</v>
       </c>
       <c r="C73" s="2" t="n">
@@ -1638,11 +1642,11 @@
       <c r="D73" s="2" t="n"/>
       <c r="E73" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="74">
+    <row r="74">
       <c r="A74" s="2" t="n">
         <v>2248</v>
       </c>
-      <c r="B74" s="2" t="n">
+      <c r="B74" s="3" t="n">
         <v>43602</v>
       </c>
       <c r="C74" s="2" t="n">
@@ -1651,11 +1655,11 @@
       <c r="D74" s="2" t="n"/>
       <c r="E74" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="75">
+    <row r="75">
       <c r="A75" s="2" t="n">
         <v>2249</v>
       </c>
-      <c r="B75" s="2" t="n">
+      <c r="B75" s="3" t="n">
         <v>43603</v>
       </c>
       <c r="C75" s="2" t="n">
@@ -1664,11 +1668,11 @@
       <c r="D75" s="2" t="n"/>
       <c r="E75" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="76">
+    <row r="76">
       <c r="A76" s="2" t="n">
         <v>2250</v>
       </c>
-      <c r="B76" s="2" t="n">
+      <c r="B76" s="3" t="n">
         <v>43603</v>
       </c>
       <c r="C76" s="2" t="n">
@@ -1677,11 +1681,11 @@
       <c r="D76" s="2" t="n"/>
       <c r="E76" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="77">
+    <row r="77">
       <c r="A77" s="2" t="n">
         <v>2251</v>
       </c>
-      <c r="B77" s="2" t="n">
+      <c r="B77" s="3" t="n">
         <v>43604</v>
       </c>
       <c r="C77" s="2" t="n">
@@ -1690,11 +1694,11 @@
       <c r="D77" s="2" t="n"/>
       <c r="E77" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="78">
+    <row r="78">
       <c r="A78" s="2" t="n">
         <v>2252</v>
       </c>
-      <c r="B78" s="2" t="n">
+      <c r="B78" s="3" t="n">
         <v>43604</v>
       </c>
       <c r="C78" s="2" t="n">
@@ -1703,11 +1707,11 @@
       <c r="D78" s="2" t="n"/>
       <c r="E78" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="79">
+    <row r="79">
       <c r="A79" s="2" t="n">
         <v>2253</v>
       </c>
-      <c r="B79" s="2" t="n">
+      <c r="B79" s="3" t="n">
         <v>43605</v>
       </c>
       <c r="C79" s="2" t="n">
@@ -1716,11 +1720,11 @@
       <c r="D79" s="2" t="n"/>
       <c r="E79" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="80">
+    <row r="80">
       <c r="A80" s="2" t="n">
         <v>2254</v>
       </c>
-      <c r="B80" s="2" t="n">
+      <c r="B80" s="3" t="n">
         <v>43606</v>
       </c>
       <c r="C80" s="2" t="n">
@@ -1729,11 +1733,11 @@
       <c r="D80" s="2" t="n"/>
       <c r="E80" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="81">
+    <row r="81">
       <c r="A81" s="2" t="n">
         <v>2255</v>
       </c>
-      <c r="B81" s="2" t="n">
+      <c r="B81" s="3" t="n">
         <v>43607</v>
       </c>
       <c r="C81" s="2" t="n">
@@ -1742,11 +1746,11 @@
       <c r="D81" s="2" t="n"/>
       <c r="E81" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="82">
+    <row r="82">
       <c r="A82" s="2" t="n">
         <v>2256</v>
       </c>
-      <c r="B82" s="2" t="n">
+      <c r="B82" s="3" t="n">
         <v>43608</v>
       </c>
       <c r="C82" s="2" t="n">
@@ -1755,11 +1759,11 @@
       <c r="D82" s="2" t="n"/>
       <c r="E82" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="83">
+    <row r="83">
       <c r="A83" s="2" t="n">
         <v>2257</v>
       </c>
-      <c r="B83" s="2" t="n">
+      <c r="B83" s="3" t="n">
         <v>43609</v>
       </c>
       <c r="C83" s="2" t="n">
@@ -1768,11 +1772,11 @@
       <c r="D83" s="2" t="n"/>
       <c r="E83" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="84">
+    <row r="84">
       <c r="A84" s="2" t="n">
         <v>2258</v>
       </c>
-      <c r="B84" s="2" t="n">
+      <c r="B84" s="3" t="n">
         <v>43610</v>
       </c>
       <c r="C84" s="2" t="n">
@@ -1781,11 +1785,11 @@
       <c r="D84" s="2" t="n"/>
       <c r="E84" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="85">
+    <row r="85">
       <c r="A85" s="2" t="n">
         <v>2259</v>
       </c>
-      <c r="B85" s="2" t="n">
+      <c r="B85" s="3" t="n">
         <v>43610</v>
       </c>
       <c r="C85" s="2" t="n">
@@ -1794,11 +1798,11 @@
       <c r="D85" s="2" t="n"/>
       <c r="E85" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="86">
+    <row r="86">
       <c r="A86" s="2" t="n">
         <v>2260</v>
       </c>
-      <c r="B86" s="2" t="n">
+      <c r="B86" s="3" t="n">
         <v>43611</v>
       </c>
       <c r="C86" s="2" t="n">
@@ -1807,11 +1811,11 @@
       <c r="D86" s="2" t="n"/>
       <c r="E86" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="87">
+    <row r="87">
       <c r="A87" s="2" t="n">
         <v>2261</v>
       </c>
-      <c r="B87" s="2" t="n">
+      <c r="B87" s="3" t="n">
         <v>43612</v>
       </c>
       <c r="C87" s="2" t="n">
@@ -1820,11 +1824,11 @@
       <c r="D87" s="2" t="n"/>
       <c r="E87" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="88">
+    <row r="88">
       <c r="A88" s="2" t="n">
         <v>2262</v>
       </c>
-      <c r="B88" s="2" t="n">
+      <c r="B88" s="3" t="n">
         <v>43612</v>
       </c>
       <c r="C88" s="2" t="n">
@@ -1833,11 +1837,11 @@
       <c r="D88" s="2" t="n"/>
       <c r="E88" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="89">
+    <row r="89">
       <c r="A89" s="2" t="n">
         <v>2263</v>
       </c>
-      <c r="B89" s="2" t="n">
+      <c r="B89" s="3" t="n">
         <v>43612</v>
       </c>
       <c r="C89" s="2" t="n">
@@ -1846,11 +1850,11 @@
       <c r="D89" s="2" t="n"/>
       <c r="E89" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="90">
+    <row r="90">
       <c r="A90" s="2" t="n">
         <v>2264</v>
       </c>
-      <c r="B90" s="2" t="n">
+      <c r="B90" s="3" t="n">
         <v>43613</v>
       </c>
       <c r="C90" s="2" t="n">
@@ -1859,11 +1863,11 @@
       <c r="D90" s="2" t="n"/>
       <c r="E90" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="91">
+    <row r="91">
       <c r="A91" s="2" t="n">
         <v>2265</v>
       </c>
-      <c r="B91" s="2" t="n">
+      <c r="B91" s="3" t="n">
         <v>43615</v>
       </c>
       <c r="C91" s="2" t="n">
@@ -1872,11 +1876,11 @@
       <c r="D91" s="2" t="n"/>
       <c r="E91" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="92">
+    <row r="92">
       <c r="A92" s="2" t="n">
         <v>2266</v>
       </c>
-      <c r="B92" s="2" t="n">
+      <c r="B92" s="3" t="n">
         <v>43615</v>
       </c>
       <c r="C92" s="2" t="n">
@@ -1885,11 +1889,11 @@
       <c r="D92" s="2" t="n"/>
       <c r="E92" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="93">
+    <row r="93">
       <c r="A93" s="2" t="n">
         <v>2267</v>
       </c>
-      <c r="B93" s="2" t="n">
+      <c r="B93" s="3" t="n">
         <v>43615</v>
       </c>
       <c r="C93" s="2" t="n">
@@ -1898,23 +1902,6 @@
       <c r="D93" s="2" t="n"/>
       <c r="E93" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="94"/>
-    <row customHeight="1" ht="18" r="95"/>
-    <row customHeight="1" ht="18" r="96"/>
-    <row customHeight="1" ht="18" r="97"/>
-    <row customHeight="1" ht="18" r="98"/>
-    <row customHeight="1" ht="18" r="99"/>
-    <row customHeight="1" ht="18" r="100"/>
-    <row customHeight="1" ht="18" r="101"/>
-    <row customHeight="1" ht="18" r="102"/>
-    <row customHeight="1" ht="18" r="103"/>
-    <row customHeight="1" ht="18" r="104"/>
-    <row customHeight="1" ht="18" r="105"/>
-    <row customHeight="1" ht="18" r="106"/>
-    <row customHeight="1" ht="18" r="107"/>
-    <row customHeight="1" ht="18" r="108"/>
-    <row customHeight="1" ht="18" r="109"/>
-    <row customHeight="1" ht="18" r="110"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1932,7 +1919,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.25" defaultRowHeight="25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -4156,7 +4143,7 @@
       <c r="G110" s="2" t="n"/>
       <c r="H110" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="111">
+    <row r="111">
       <c r="A111" s="2" t="n">
         <v>39</v>
       </c>
@@ -4176,7 +4163,7 @@
       <c r="G111" s="2" t="n"/>
       <c r="H111" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="112">
+    <row r="112">
       <c r="A112" s="2" t="n">
         <v>40</v>
       </c>
@@ -4196,7 +4183,7 @@
       <c r="G112" s="2" t="n"/>
       <c r="H112" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="113">
+    <row r="113">
       <c r="A113" s="2" t="n">
         <v>41</v>
       </c>
@@ -4216,7 +4203,7 @@
       <c r="G113" s="2" t="n"/>
       <c r="H113" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="114">
+    <row r="114">
       <c r="A114" s="2" t="n">
         <v>43</v>
       </c>
@@ -4236,7 +4223,7 @@
       <c r="G114" s="2" t="n"/>
       <c r="H114" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="115">
+    <row r="115">
       <c r="A115" s="2" t="n">
         <v>42</v>
       </c>
@@ -4256,7 +4243,7 @@
       <c r="G115" s="2" t="n"/>
       <c r="H115" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="116">
+    <row r="116">
       <c r="A116" s="2" t="n">
         <v>44</v>
       </c>
@@ -4276,7 +4263,7 @@
       <c r="G116" s="2" t="n"/>
       <c r="H116" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="117">
+    <row r="117">
       <c r="A117" s="2" t="n">
         <v>45</v>
       </c>
@@ -4296,7 +4283,7 @@
       <c r="G117" s="2" t="n"/>
       <c r="H117" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="118">
+    <row r="118">
       <c r="A118" s="2" t="n">
         <v>46</v>
       </c>
@@ -4316,7 +4303,7 @@
       <c r="G118" s="2" t="n"/>
       <c r="H118" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="119">
+    <row r="119">
       <c r="A119" s="2" t="n">
         <v>47</v>
       </c>
@@ -4336,7 +4323,7 @@
       <c r="G119" s="2" t="n"/>
       <c r="H119" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="120">
+    <row r="120">
       <c r="A120" s="2" t="n">
         <v>48</v>
       </c>
@@ -4356,7 +4343,7 @@
       <c r="G120" s="2" t="n"/>
       <c r="H120" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="121">
+    <row r="121">
       <c r="A121" s="2" t="n">
         <v>49</v>
       </c>
@@ -4376,7 +4363,7 @@
       <c r="G121" s="2" t="n"/>
       <c r="H121" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="122">
+    <row r="122">
       <c r="A122" s="2" t="n">
         <v>50</v>
       </c>
@@ -4396,7 +4383,7 @@
       <c r="G122" s="2" t="n"/>
       <c r="H122" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="123">
+    <row r="123">
       <c r="A123" s="2" t="n">
         <v>51</v>
       </c>
@@ -4416,7 +4403,7 @@
       <c r="G123" s="2" t="n"/>
       <c r="H123" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="124">
+    <row r="124">
       <c r="A124" s="2" t="n">
         <v>52</v>
       </c>
@@ -4436,7 +4423,7 @@
       <c r="G124" s="2" t="n"/>
       <c r="H124" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="125">
+    <row r="125">
       <c r="A125" s="2" t="n">
         <v>53</v>
       </c>
@@ -4456,7 +4443,7 @@
       <c r="G125" s="2" t="n"/>
       <c r="H125" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="126">
+    <row r="126">
       <c r="A126" s="2" t="n">
         <v>54</v>
       </c>
@@ -4476,7 +4463,7 @@
       <c r="G126" s="2" t="n"/>
       <c r="H126" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="127">
+    <row r="127">
       <c r="A127" s="2" t="n">
         <v>55</v>
       </c>
@@ -4496,7 +4483,7 @@
       <c r="G127" s="2" t="n"/>
       <c r="H127" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="128">
+    <row r="128">
       <c r="A128" s="2" t="n">
         <v>56</v>
       </c>
@@ -4516,7 +4503,7 @@
       <c r="G128" s="2" t="n"/>
       <c r="H128" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="129">
+    <row r="129">
       <c r="A129" s="2" t="n">
         <v>57</v>
       </c>
@@ -4536,7 +4523,7 @@
       <c r="G129" s="2" t="n"/>
       <c r="H129" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="130">
+    <row r="130">
       <c r="A130" s="2" t="n">
         <v>58</v>
       </c>
@@ -4556,7 +4543,7 @@
       <c r="G130" s="2" t="n"/>
       <c r="H130" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="131">
+    <row r="131">
       <c r="A131" s="2" t="n">
         <v>59</v>
       </c>
@@ -4576,7 +4563,7 @@
       <c r="G131" s="2" t="n"/>
       <c r="H131" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="132">
+    <row r="132">
       <c r="A132" s="2" t="n">
         <v>60</v>
       </c>
@@ -4596,7 +4583,7 @@
       <c r="G132" s="2" t="n"/>
       <c r="H132" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="133">
+    <row r="133">
       <c r="A133" s="2" t="n">
         <v>61</v>
       </c>
@@ -4616,7 +4603,7 @@
       <c r="G133" s="2" t="n"/>
       <c r="H133" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="134">
+    <row r="134">
       <c r="A134" s="2" t="n">
         <v>62</v>
       </c>
@@ -4636,7 +4623,7 @@
       <c r="G134" s="2" t="n"/>
       <c r="H134" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="135">
+    <row r="135">
       <c r="A135" s="2" t="n">
         <v>63</v>
       </c>
@@ -4656,7 +4643,7 @@
       <c r="G135" s="2" t="n"/>
       <c r="H135" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="136">
+    <row r="136">
       <c r="A136" s="2" t="n">
         <v>64</v>
       </c>
@@ -4676,7 +4663,7 @@
       <c r="G136" s="2" t="n"/>
       <c r="H136" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="137">
+    <row r="137">
       <c r="A137" s="2" t="n">
         <v>65</v>
       </c>
@@ -4696,7 +4683,7 @@
       <c r="G137" s="2" t="n"/>
       <c r="H137" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="138">
+    <row r="138">
       <c r="A138" s="2" t="n">
         <v>66</v>
       </c>
@@ -4716,7 +4703,7 @@
       <c r="G138" s="2" t="n"/>
       <c r="H138" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="139">
+    <row r="139">
       <c r="A139" s="2" t="n">
         <v>69</v>
       </c>
@@ -4736,7 +4723,7 @@
       <c r="G139" s="2" t="n"/>
       <c r="H139" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="140">
+    <row r="140">
       <c r="A140" s="2" t="n">
         <v>70</v>
       </c>
@@ -4756,7 +4743,7 @@
       <c r="G140" s="2" t="n"/>
       <c r="H140" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="141">
+    <row r="141">
       <c r="A141" s="2" t="n">
         <v>67</v>
       </c>
@@ -4776,7 +4763,7 @@
       <c r="G141" s="2" t="n"/>
       <c r="H141" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="142">
+    <row r="142">
       <c r="A142" s="2" t="n">
         <v>68</v>
       </c>
@@ -4796,7 +4783,7 @@
       <c r="G142" s="2" t="n"/>
       <c r="H142" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="143">
+    <row r="143">
       <c r="A143" s="2" t="n">
         <v>71</v>
       </c>
@@ -4816,116 +4803,6 @@
       <c r="G143" s="2" t="n"/>
       <c r="H143" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="144"/>
-    <row customHeight="1" ht="18" r="145"/>
-    <row customHeight="1" ht="18" r="146"/>
-    <row customHeight="1" ht="18" r="147"/>
-    <row customHeight="1" ht="18" r="148"/>
-    <row customHeight="1" ht="18" r="149"/>
-    <row customHeight="1" ht="18" r="150"/>
-    <row customHeight="1" ht="18" r="151"/>
-    <row customHeight="1" ht="18" r="152"/>
-    <row customHeight="1" ht="18" r="153"/>
-    <row customHeight="1" ht="18" r="154"/>
-    <row customHeight="1" ht="18" r="155"/>
-    <row customHeight="1" ht="18" r="156"/>
-    <row customHeight="1" ht="18" r="157"/>
-    <row customHeight="1" ht="18" r="158"/>
-    <row customHeight="1" ht="18" r="159"/>
-    <row customHeight="1" ht="18" r="160"/>
-    <row customHeight="1" ht="18" r="161"/>
-    <row customHeight="1" ht="18" r="162"/>
-    <row customHeight="1" ht="18" r="163"/>
-    <row customHeight="1" ht="18" r="164"/>
-    <row customHeight="1" ht="18" r="165"/>
-    <row customHeight="1" ht="18" r="166"/>
-    <row customHeight="1" ht="18" r="167"/>
-    <row customHeight="1" ht="18" r="168"/>
-    <row customHeight="1" ht="18" r="169"/>
-    <row customHeight="1" ht="18" r="170"/>
-    <row customHeight="1" ht="18" r="171"/>
-    <row customHeight="1" ht="18" r="172"/>
-    <row customHeight="1" ht="18" r="173"/>
-    <row customHeight="1" ht="18" r="174"/>
-    <row customHeight="1" ht="18" r="175"/>
-    <row customHeight="1" ht="18" r="176"/>
-    <row customHeight="1" ht="18" r="177"/>
-    <row customHeight="1" ht="18" r="178"/>
-    <row customHeight="1" ht="18" r="179"/>
-    <row customHeight="1" ht="18" r="180"/>
-    <row customHeight="1" ht="18" r="181"/>
-    <row customHeight="1" ht="18" r="182"/>
-    <row customHeight="1" ht="18" r="183"/>
-    <row customHeight="1" ht="18" r="184"/>
-    <row customHeight="1" ht="18" r="185"/>
-    <row customHeight="1" ht="18" r="186"/>
-    <row customHeight="1" ht="18" r="187"/>
-    <row customHeight="1" ht="18" r="188"/>
-    <row customHeight="1" ht="18" r="189"/>
-    <row customHeight="1" ht="18" r="190"/>
-    <row customHeight="1" ht="18" r="191"/>
-    <row customHeight="1" ht="18" r="192"/>
-    <row customHeight="1" ht="18" r="193"/>
-    <row customHeight="1" ht="18" r="194"/>
-    <row customHeight="1" ht="18" r="195"/>
-    <row customHeight="1" ht="18" r="196"/>
-    <row customHeight="1" ht="18" r="197"/>
-    <row customHeight="1" ht="18" r="198"/>
-    <row customHeight="1" ht="18" r="199"/>
-    <row customHeight="1" ht="18" r="200"/>
-    <row customHeight="1" ht="18" r="201"/>
-    <row customHeight="1" ht="18" r="202"/>
-    <row customHeight="1" ht="18" r="203"/>
-    <row customHeight="1" ht="18" r="204"/>
-    <row customHeight="1" ht="18" r="205"/>
-    <row customHeight="1" ht="18" r="206"/>
-    <row customHeight="1" ht="18" r="207"/>
-    <row customHeight="1" ht="18" r="208"/>
-    <row customHeight="1" ht="18" r="209"/>
-    <row customHeight="1" ht="18" r="210"/>
-    <row customHeight="1" ht="18" r="211"/>
-    <row customHeight="1" ht="18" r="212"/>
-    <row customHeight="1" ht="18" r="213"/>
-    <row customHeight="1" ht="18" r="214"/>
-    <row customHeight="1" ht="18" r="215"/>
-    <row customHeight="1" ht="18" r="216"/>
-    <row customHeight="1" ht="18" r="217"/>
-    <row customHeight="1" ht="18" r="218"/>
-    <row customHeight="1" ht="18" r="219"/>
-    <row customHeight="1" ht="18" r="220"/>
-    <row customHeight="1" ht="18" r="221"/>
-    <row customHeight="1" ht="18" r="222"/>
-    <row customHeight="1" ht="18" r="223"/>
-    <row customHeight="1" ht="18" r="224"/>
-    <row customHeight="1" ht="18" r="225"/>
-    <row customHeight="1" ht="18" r="226"/>
-    <row customHeight="1" ht="18" r="227"/>
-    <row customHeight="1" ht="18" r="228"/>
-    <row customHeight="1" ht="18" r="229"/>
-    <row customHeight="1" ht="18" r="230"/>
-    <row customHeight="1" ht="18" r="231"/>
-    <row customHeight="1" ht="18" r="232"/>
-    <row customHeight="1" ht="18" r="233"/>
-    <row customHeight="1" ht="18" r="234"/>
-    <row customHeight="1" ht="18" r="235"/>
-    <row customHeight="1" ht="18" r="236"/>
-    <row customHeight="1" ht="18" r="237"/>
-    <row customHeight="1" ht="18" r="238"/>
-    <row customHeight="1" ht="18" r="239"/>
-    <row customHeight="1" ht="18" r="240"/>
-    <row customHeight="1" ht="18" r="241"/>
-    <row customHeight="1" ht="18" r="242"/>
-    <row customHeight="1" ht="18" r="243"/>
-    <row customHeight="1" ht="18" r="244"/>
-    <row customHeight="1" ht="18" r="245"/>
-    <row customHeight="1" ht="18" r="246"/>
-    <row customHeight="1" ht="18" r="247"/>
-    <row customHeight="1" ht="18" r="248"/>
-    <row customHeight="1" ht="18" r="249"/>
-    <row customHeight="1" ht="18" r="250"/>
-    <row customHeight="1" ht="18" r="251"/>
-    <row customHeight="1" ht="18" r="252"/>
-    <row customHeight="1" ht="18" r="253"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -4943,7 +4820,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.25" defaultRowHeight="25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -5095,15 +4972,6 @@
         <v>20</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="254"/>
-    <row customHeight="1" ht="18" r="255"/>
-    <row customHeight="1" ht="18" r="256"/>
-    <row customHeight="1" ht="18" r="257"/>
-    <row customHeight="1" ht="18" r="258"/>
-    <row customHeight="1" ht="18" r="259"/>
-    <row customHeight="1" ht="18" r="260"/>
-    <row customHeight="1" ht="18" r="261"/>
-    <row customHeight="1" ht="18" r="262"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
set default column width: all columns' data now visible without the need for manual adjustment
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -375,7 +375,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14" defaultRowHeight="18"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -685,7 +685,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14" defaultRowHeight="18"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1919,7 +1919,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14" defaultRowHeight="18"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -4820,7 +4820,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14" defaultRowHeight="18"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
added successful merge message; cleaned code a bit & improved variable names; enhanced comments
</commit_message>
<xml_diff>
--- a/Comp230/merged_sales_data.xlsx
+++ b/Comp230/merged_sales_data.xlsx
@@ -38,7 +38,7 @@
     <font>
       <name val="Arial"/>
       <b val="1"/>
-      <sz val="12"/>
+      <sz val="13"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,9 +72,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="basic" xfId="1"/>
-    <cellStyle hidden="0" name="basic_bold" xfId="2"/>
-    <cellStyle hidden="0" name="date_style" xfId="3"/>
+    <cellStyle hidden="0" name="default_cell" xfId="1"/>
+    <cellStyle hidden="0" name="bold_header" xfId="2"/>
+    <cellStyle hidden="0" name="date_cell" xfId="3"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -369,7 +369,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -393,8 +393,6 @@
           <t>Last</t>
         </is>
       </c>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -410,8 +408,6 @@
           <t>Wang</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -427,8 +423,6 @@
           <t>Wang</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n"/>
-      <c r="E3" s="2" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -444,8 +438,6 @@
           <t>Kondrat</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -461,8 +453,6 @@
           <t>Hussain</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -478,8 +468,6 @@
           <t>Wang</t>
         </is>
       </c>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -495,8 +483,6 @@
           <t>Ford</t>
         </is>
       </c>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -512,8 +498,6 @@
           <t>It</t>
         </is>
       </c>
-      <c r="D8" s="2" t="n"/>
-      <c r="E8" s="2" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -529,8 +513,6 @@
           <t>Rocks</t>
         </is>
       </c>
-      <c r="D9" s="2" t="n"/>
-      <c r="E9" s="2" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -546,8 +528,6 @@
           <t>Sugar</t>
         </is>
       </c>
-      <c r="D10" s="2" t="n"/>
-      <c r="E10" s="2" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -563,8 +543,6 @@
           <t>Python</t>
         </is>
       </c>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" s="2" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -580,8 +558,6 @@
           <t>Winger</t>
         </is>
       </c>
-      <c r="D12" s="2" t="n"/>
-      <c r="E12" s="2" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -597,8 +573,6 @@
           <t>Ford</t>
         </is>
       </c>
-      <c r="D13" s="2" t="n"/>
-      <c r="E13" s="2" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -614,8 +588,6 @@
           <t>Parker</t>
         </is>
       </c>
-      <c r="D14" s="2" t="n"/>
-      <c r="E14" s="2" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -631,8 +603,6 @@
           <t>Stark</t>
         </is>
       </c>
-      <c r="D15" s="2" t="n"/>
-      <c r="E15" s="2" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -648,8 +618,6 @@
           <t>Banner</t>
         </is>
       </c>
-      <c r="D16" s="2" t="n"/>
-      <c r="E16" s="2" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -665,8 +633,6 @@
           <t>Danvers</t>
         </is>
       </c>
-      <c r="D17" s="2" t="n"/>
-      <c r="E17" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -679,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -703,8 +669,6 @@
           <t>Customer</t>
         </is>
       </c>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -716,8 +680,6 @@
       <c r="C2" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -729,8 +691,6 @@
       <c r="C3" s="2" t="n">
         <v>133</v>
       </c>
-      <c r="D3" s="2" t="n"/>
-      <c r="E3" s="2" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -742,8 +702,6 @@
       <c r="C4" s="2" t="n">
         <v>131</v>
       </c>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -755,8 +713,6 @@
       <c r="C5" s="2" t="n">
         <v>131</v>
       </c>
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -768,8 +724,6 @@
       <c r="C6" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -781,8 +735,6 @@
       <c r="C7" s="2" t="n">
         <v>133</v>
       </c>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -794,8 +746,6 @@
       <c r="C8" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="D8" s="2" t="n"/>
-      <c r="E8" s="2" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -807,8 +757,6 @@
       <c r="C9" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="D9" s="2" t="n"/>
-      <c r="E9" s="2" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -820,8 +768,6 @@
       <c r="C10" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="D10" s="2" t="n"/>
-      <c r="E10" s="2" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -833,8 +779,6 @@
       <c r="C11" s="2" t="n">
         <v>129</v>
       </c>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" s="2" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -846,8 +790,6 @@
       <c r="C12" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="D12" s="2" t="n"/>
-      <c r="E12" s="2" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -859,8 +801,6 @@
       <c r="C13" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="D13" s="2" t="n"/>
-      <c r="E13" s="2" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -872,8 +812,6 @@
       <c r="C14" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="D14" s="2" t="n"/>
-      <c r="E14" s="2" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -885,8 +823,6 @@
       <c r="C15" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="D15" s="2" t="n"/>
-      <c r="E15" s="2" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -898,8 +834,6 @@
       <c r="C16" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="D16" s="2" t="n"/>
-      <c r="E16" s="2" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -911,8 +845,6 @@
       <c r="C17" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="D17" s="2" t="n"/>
-      <c r="E17" s="2" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -924,8 +856,6 @@
       <c r="C18" s="2" t="n">
         <v>132</v>
       </c>
-      <c r="D18" s="2" t="n"/>
-      <c r="E18" s="2" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -937,8 +867,6 @@
       <c r="C19" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="D19" s="2" t="n"/>
-      <c r="E19" s="2" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -950,8 +878,6 @@
       <c r="C20" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="D20" s="2" t="n"/>
-      <c r="E20" s="2" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -963,8 +889,6 @@
       <c r="C21" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="D21" s="2" t="n"/>
-      <c r="E21" s="2" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -976,8 +900,6 @@
       <c r="C22" s="2" t="n">
         <v>131</v>
       </c>
-      <c r="D22" s="2" t="n"/>
-      <c r="E22" s="2" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -989,8 +911,6 @@
       <c r="C23" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="D23" s="2" t="n"/>
-      <c r="E23" s="2" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -1002,8 +922,6 @@
       <c r="C24" s="2" t="n">
         <v>134</v>
       </c>
-      <c r="D24" s="2" t="n"/>
-      <c r="E24" s="2" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -1015,8 +933,6 @@
       <c r="C25" s="2" t="n">
         <v>129</v>
       </c>
-      <c r="D25" s="2" t="n"/>
-      <c r="E25" s="2" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -1028,8 +944,6 @@
       <c r="C26" s="2" t="n">
         <v>134</v>
       </c>
-      <c r="D26" s="2" t="n"/>
-      <c r="E26" s="2" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -1041,8 +955,6 @@
       <c r="C27" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="D27" s="2" t="n"/>
-      <c r="E27" s="2" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -1054,8 +966,6 @@
       <c r="C28" s="2" t="n">
         <v>131</v>
       </c>
-      <c r="D28" s="2" t="n"/>
-      <c r="E28" s="2" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -1067,8 +977,6 @@
       <c r="C29" s="2" t="n">
         <v>132</v>
       </c>
-      <c r="D29" s="2" t="n"/>
-      <c r="E29" s="2" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -1080,8 +988,6 @@
       <c r="C30" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="D30" s="2" t="n"/>
-      <c r="E30" s="2" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -1093,8 +999,6 @@
       <c r="C31" s="2" t="n">
         <v>132</v>
       </c>
-      <c r="D31" s="2" t="n"/>
-      <c r="E31" s="2" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1106,8 +1010,6 @@
       <c r="C32" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="D32" s="2" t="n"/>
-      <c r="E32" s="2" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -1119,8 +1021,6 @@
       <c r="C33" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="D33" s="2" t="n"/>
-      <c r="E33" s="2" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -1132,8 +1032,6 @@
       <c r="C34" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="D34" s="2" t="n"/>
-      <c r="E34" s="2" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -1145,8 +1043,6 @@
       <c r="C35" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="D35" s="2" t="n"/>
-      <c r="E35" s="2" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -1158,8 +1054,6 @@
       <c r="C36" s="2" t="n">
         <v>129</v>
       </c>
-      <c r="D36" s="2" t="n"/>
-      <c r="E36" s="2" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -1171,8 +1065,6 @@
       <c r="C37" s="2" t="n">
         <v>129</v>
       </c>
-      <c r="D37" s="2" t="n"/>
-      <c r="E37" s="2" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -1184,8 +1076,6 @@
       <c r="C38" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="D38" s="2" t="n"/>
-      <c r="E38" s="2" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -1197,8 +1087,6 @@
       <c r="C39" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="D39" s="2" t="n"/>
-      <c r="E39" s="2" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -1210,8 +1098,6 @@
       <c r="C40" s="2" t="n">
         <v>134</v>
       </c>
-      <c r="D40" s="2" t="n"/>
-      <c r="E40" s="2" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -1223,8 +1109,6 @@
       <c r="C41" s="2" t="n">
         <v>132</v>
       </c>
-      <c r="D41" s="2" t="n"/>
-      <c r="E41" s="2" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -1236,8 +1120,6 @@
       <c r="C42" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="D42" s="2" t="n"/>
-      <c r="E42" s="2" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -1249,8 +1131,6 @@
       <c r="C43" s="2" t="n">
         <v>133</v>
       </c>
-      <c r="D43" s="2" t="n"/>
-      <c r="E43" s="2" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -1262,8 +1142,6 @@
       <c r="C44" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="D44" s="2" t="n"/>
-      <c r="E44" s="2" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -1275,8 +1153,6 @@
       <c r="C45" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="D45" s="2" t="n"/>
-      <c r="E45" s="2" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -1288,8 +1164,6 @@
       <c r="C46" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="D46" s="2" t="n"/>
-      <c r="E46" s="2" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -1301,8 +1175,6 @@
       <c r="C47" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="D47" s="2" t="n"/>
-      <c r="E47" s="2" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -1314,8 +1186,6 @@
       <c r="C48" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="D48" s="2" t="n"/>
-      <c r="E48" s="2" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -1327,8 +1197,6 @@
       <c r="C49" s="2" t="n">
         <v>1002</v>
       </c>
-      <c r="D49" s="2" t="n"/>
-      <c r="E49" s="2" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -1340,8 +1208,6 @@
       <c r="C50" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="D50" s="2" t="n"/>
-      <c r="E50" s="2" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
@@ -1353,8 +1219,6 @@
       <c r="C51" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="D51" s="2" t="n"/>
-      <c r="E51" s="2" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -1366,8 +1230,6 @@
       <c r="C52" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="D52" s="2" t="n"/>
-      <c r="E52" s="2" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -1379,8 +1241,6 @@
       <c r="C53" s="2" t="n">
         <v>1002</v>
       </c>
-      <c r="D53" s="2" t="n"/>
-      <c r="E53" s="2" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -1392,8 +1252,6 @@
       <c r="C54" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="D54" s="2" t="n"/>
-      <c r="E54" s="2" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
@@ -1405,8 +1263,6 @@
       <c r="C55" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="D55" s="2" t="n"/>
-      <c r="E55" s="2" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
@@ -1418,8 +1274,6 @@
       <c r="C56" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="D56" s="2" t="n"/>
-      <c r="E56" s="2" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
@@ -1431,8 +1285,6 @@
       <c r="C57" s="2" t="n">
         <v>129</v>
       </c>
-      <c r="D57" s="2" t="n"/>
-      <c r="E57" s="2" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
@@ -1444,8 +1296,6 @@
       <c r="C58" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="D58" s="2" t="n"/>
-      <c r="E58" s="2" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
@@ -1457,8 +1307,6 @@
       <c r="C59" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="D59" s="2" t="n"/>
-      <c r="E59" s="2" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
@@ -1470,8 +1318,6 @@
       <c r="C60" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="D60" s="2" t="n"/>
-      <c r="E60" s="2" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
@@ -1483,8 +1329,6 @@
       <c r="C61" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="D61" s="2" t="n"/>
-      <c r="E61" s="2" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
@@ -1496,8 +1340,6 @@
       <c r="C62" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="D62" s="2" t="n"/>
-      <c r="E62" s="2" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -1509,8 +1351,6 @@
       <c r="C63" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="D63" s="2" t="n"/>
-      <c r="E63" s="2" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
@@ -1522,8 +1362,6 @@
       <c r="C64" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="D64" s="2" t="n"/>
-      <c r="E64" s="2" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
@@ -1535,8 +1373,6 @@
       <c r="C65" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="D65" s="2" t="n"/>
-      <c r="E65" s="2" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
@@ -1548,8 +1384,6 @@
       <c r="C66" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="D66" s="2" t="n"/>
-      <c r="E66" s="2" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
@@ -1561,8 +1395,6 @@
       <c r="C67" s="2" t="n">
         <v>127</v>
       </c>
-      <c r="D67" s="2" t="n"/>
-      <c r="E67" s="2" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
@@ -1574,8 +1406,6 @@
       <c r="C68" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="D68" s="2" t="n"/>
-      <c r="E68" s="2" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
@@ -1587,8 +1417,6 @@
       <c r="C69" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="D69" s="2" t="n"/>
-      <c r="E69" s="2" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
@@ -1600,8 +1428,6 @@
       <c r="C70" s="2" t="n">
         <v>1003</v>
       </c>
-      <c r="D70" s="2" t="n"/>
-      <c r="E70" s="2" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
@@ -1613,8 +1439,6 @@
       <c r="C71" s="2" t="n">
         <v>129</v>
       </c>
-      <c r="D71" s="2" t="n"/>
-      <c r="E71" s="2" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
@@ -1626,8 +1450,6 @@
       <c r="C72" s="2" t="n">
         <v>1003</v>
       </c>
-      <c r="D72" s="2" t="n"/>
-      <c r="E72" s="2" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
@@ -1639,8 +1461,6 @@
       <c r="C73" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="D73" s="2" t="n"/>
-      <c r="E73" s="2" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
@@ -1652,8 +1472,6 @@
       <c r="C74" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="D74" s="2" t="n"/>
-      <c r="E74" s="2" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
@@ -1665,8 +1483,6 @@
       <c r="C75" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="D75" s="2" t="n"/>
-      <c r="E75" s="2" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
@@ -1678,8 +1494,6 @@
       <c r="C76" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="D76" s="2" t="n"/>
-      <c r="E76" s="2" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
@@ -1691,8 +1505,6 @@
       <c r="C77" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="D77" s="2" t="n"/>
-      <c r="E77" s="2" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -1704,8 +1516,6 @@
       <c r="C78" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="D78" s="2" t="n"/>
-      <c r="E78" s="2" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
@@ -1717,8 +1527,6 @@
       <c r="C79" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="D79" s="2" t="n"/>
-      <c r="E79" s="2" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
@@ -1730,8 +1538,6 @@
       <c r="C80" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="D80" s="2" t="n"/>
-      <c r="E80" s="2" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
@@ -1743,8 +1549,6 @@
       <c r="C81" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="D81" s="2" t="n"/>
-      <c r="E81" s="2" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
@@ -1756,8 +1560,6 @@
       <c r="C82" s="2" t="n">
         <v>129</v>
       </c>
-      <c r="D82" s="2" t="n"/>
-      <c r="E82" s="2" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
@@ -1769,8 +1571,6 @@
       <c r="C83" s="2" t="n">
         <v>129</v>
       </c>
-      <c r="D83" s="2" t="n"/>
-      <c r="E83" s="2" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
@@ -1782,8 +1582,6 @@
       <c r="C84" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="D84" s="2" t="n"/>
-      <c r="E84" s="2" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
@@ -1795,8 +1593,6 @@
       <c r="C85" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="D85" s="2" t="n"/>
-      <c r="E85" s="2" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
@@ -1808,8 +1604,6 @@
       <c r="C86" s="2" t="n">
         <v>1003</v>
       </c>
-      <c r="D86" s="2" t="n"/>
-      <c r="E86" s="2" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
@@ -1821,8 +1615,6 @@
       <c r="C87" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="D87" s="2" t="n"/>
-      <c r="E87" s="2" t="n"/>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
@@ -1834,8 +1626,6 @@
       <c r="C88" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="D88" s="2" t="n"/>
-      <c r="E88" s="2" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
@@ -1847,8 +1637,6 @@
       <c r="C89" s="2" t="n">
         <v>1002</v>
       </c>
-      <c r="D89" s="2" t="n"/>
-      <c r="E89" s="2" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
@@ -1860,8 +1648,6 @@
       <c r="C90" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="D90" s="2" t="n"/>
-      <c r="E90" s="2" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
@@ -1873,8 +1659,6 @@
       <c r="C91" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="D91" s="2" t="n"/>
-      <c r="E91" s="2" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
@@ -1886,8 +1670,6 @@
       <c r="C92" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="D92" s="2" t="n"/>
-      <c r="E92" s="2" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
@@ -1899,8 +1681,6 @@
       <c r="C93" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="D93" s="2" t="n"/>
-      <c r="E93" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1989,11 +1769,7 @@
         <v>180</v>
       </c>
       <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>Total of all invoices</t>
-        </is>
-      </c>
+      <c r="H3" s="2" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -2013,9 +1789,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="2" t="n"/>
-      <c r="H4" s="2" t="n">
-        <v>15020</v>
-      </c>
+      <c r="H4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -2259,40 +2033,40 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>228</v>
       </c>
       <c r="C17" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="n">
         <v>6</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>5</v>
       </c>
       <c r="E17" s="2" t="n"/>
       <c r="F17" s="2" t="n">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="G17" s="2" t="n"/>
       <c r="H17" s="2" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>228</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="2" t="n"/>
       <c r="F18" s="2" t="n">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="G18" s="2" t="n"/>
       <c r="H18" s="2" t="n"/>
@@ -2559,60 +2333,60 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>238</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E32" s="2" t="n"/>
       <c r="F32" s="2" t="n">
-        <v>60</v>
+        <v>270</v>
       </c>
       <c r="G32" s="2" t="n"/>
       <c r="H32" s="2" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>238</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E33" s="2" t="n"/>
       <c r="F33" s="2" t="n">
-        <v>270</v>
+        <v>60</v>
       </c>
       <c r="G33" s="2" t="n"/>
       <c r="H33" s="2" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>239</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E34" s="2" t="n"/>
       <c r="F34" s="2" t="n">
-        <v>450</v>
+        <v>100</v>
       </c>
       <c r="G34" s="2" t="n"/>
       <c r="H34" s="2" t="n"/>
@@ -2639,20 +2413,20 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>239</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E36" s="2" t="n"/>
       <c r="F36" s="2" t="n">
-        <v>100</v>
+        <v>450</v>
       </c>
       <c r="G36" s="2" t="n"/>
       <c r="H36" s="2" t="n"/>
@@ -3279,36 +3053,36 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B68" s="2" t="n">
         <v>267</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D68" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E68" s="2" t="n"/>
       <c r="F68" s="2" t="n">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="G68" s="2" t="n"/>
       <c r="H68" s="2" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2" t="n">
         <v>267</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D69" s="2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E69" s="2" t="n"/>
       <c r="F69" s="2" t="n">
@@ -3319,67 +3093,67 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70" s="2" t="n">
         <v>267</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D70" s="2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E70" s="2" t="n"/>
       <c r="F70" s="2" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G70" s="2" t="n"/>
       <c r="H70" s="2" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>267</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D71" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E71" s="2" t="n"/>
       <c r="F71" s="2" t="n">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="G71" s="2" t="n"/>
       <c r="H71" s="2" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B72" s="2" t="n">
         <v>267</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E72" s="2" t="n"/>
       <c r="F72" s="2" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G72" s="2" t="n"/>
       <c r="H72" s="2" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>1</v>
+        <v>1001</v>
       </c>
       <c r="B73" s="2" t="n">
         <v>2222</v>
@@ -3399,7 +3173,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>2</v>
+        <v>1002</v>
       </c>
       <c r="B74" s="2" t="n">
         <v>2222</v>
@@ -3415,15 +3189,11 @@
         <v>560</v>
       </c>
       <c r="G74" s="2" t="n"/>
-      <c r="H74" s="2" t="inlineStr">
-        <is>
-          <t>Total of all invoices</t>
-        </is>
-      </c>
+      <c r="H74" s="2" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>3</v>
+        <v>1003</v>
       </c>
       <c r="B75" s="2" t="n">
         <v>2222</v>
@@ -3439,13 +3209,11 @@
         <v>40</v>
       </c>
       <c r="G75" s="2" t="n"/>
-      <c r="H75" s="2" t="n">
-        <v>16350</v>
-      </c>
+      <c r="H75" s="2" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>4</v>
+        <v>1004</v>
       </c>
       <c r="B76" s="2" t="n">
         <v>2222</v>
@@ -3465,87 +3233,87 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>8</v>
+        <v>1005</v>
       </c>
       <c r="B77" s="2" t="n">
         <v>2223</v>
       </c>
       <c r="C77" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D77" s="2" t="n">
         <v>2</v>
-      </c>
-      <c r="D77" s="2" t="n">
-        <v>3</v>
       </c>
       <c r="E77" s="2" t="n"/>
       <c r="F77" s="2" t="n">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="G77" s="2" t="n"/>
       <c r="H77" s="2" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>7</v>
+        <v>1006</v>
       </c>
       <c r="B78" s="2" t="n">
         <v>2223</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D78" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E78" s="2" t="n"/>
       <c r="F78" s="2" t="n">
-        <v>280</v>
+        <v>420</v>
       </c>
       <c r="G78" s="2" t="n"/>
       <c r="H78" s="2" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>5</v>
+        <v>1007</v>
       </c>
       <c r="B79" s="2" t="n">
         <v>2223</v>
       </c>
       <c r="C79" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D79" s="2" t="n">
         <v>7</v>
-      </c>
-      <c r="D79" s="2" t="n">
-        <v>2</v>
       </c>
       <c r="E79" s="2" t="n"/>
       <c r="F79" s="2" t="n">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="G79" s="2" t="n"/>
       <c r="H79" s="2" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>6</v>
+        <v>1008</v>
       </c>
       <c r="B80" s="2" t="n">
         <v>2223</v>
       </c>
       <c r="C80" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D80" s="2" t="n">
         <v>3</v>
-      </c>
-      <c r="D80" s="2" t="n">
-        <v>6</v>
       </c>
       <c r="E80" s="2" t="n"/>
       <c r="F80" s="2" t="n">
-        <v>420</v>
+        <v>90</v>
       </c>
       <c r="G80" s="2" t="n"/>
       <c r="H80" s="2" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>9</v>
+        <v>1009</v>
       </c>
       <c r="B81" s="2" t="n">
         <v>2224</v>
@@ -3565,7 +3333,7 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>10</v>
+        <v>1010</v>
       </c>
       <c r="B82" s="2" t="n">
         <v>2224</v>
@@ -3585,7 +3353,7 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>11</v>
+        <v>1011</v>
       </c>
       <c r="B83" s="2" t="n">
         <v>2225</v>
@@ -3605,7 +3373,7 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>12</v>
+        <v>1012</v>
       </c>
       <c r="B84" s="2" t="n">
         <v>2225</v>
@@ -3625,7 +3393,7 @@
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>13</v>
+        <v>1013</v>
       </c>
       <c r="B85" s="2" t="n">
         <v>2226</v>
@@ -3645,7 +3413,7 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>14</v>
+        <v>1014</v>
       </c>
       <c r="B86" s="2" t="n">
         <v>2226</v>
@@ -3665,7 +3433,7 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>15</v>
+        <v>1015</v>
       </c>
       <c r="B87" s="2" t="n">
         <v>2227</v>
@@ -3685,47 +3453,47 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>17</v>
+        <v>1016</v>
       </c>
       <c r="B88" s="2" t="n">
         <v>2228</v>
       </c>
       <c r="C88" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D88" s="2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E88" s="2" t="n"/>
       <c r="F88" s="2" t="n">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="G88" s="2" t="n"/>
       <c r="H88" s="2" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>16</v>
+        <v>1017</v>
       </c>
       <c r="B89" s="2" t="n">
         <v>2228</v>
       </c>
       <c r="C89" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D89" s="2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E89" s="2" t="n"/>
       <c r="F89" s="2" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="G89" s="2" t="n"/>
       <c r="H89" s="2" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>18</v>
+        <v>1018</v>
       </c>
       <c r="B90" s="2" t="n">
         <v>2229</v>
@@ -3745,7 +3513,7 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>19</v>
+        <v>1019</v>
       </c>
       <c r="B91" s="2" t="n">
         <v>2229</v>
@@ -3765,7 +3533,7 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>20</v>
+        <v>1020</v>
       </c>
       <c r="B92" s="2" t="n">
         <v>2229</v>
@@ -3785,7 +3553,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>21</v>
+        <v>1021</v>
       </c>
       <c r="B93" s="2" t="n">
         <v>2230</v>
@@ -3805,7 +3573,7 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>22</v>
+        <v>1022</v>
       </c>
       <c r="B94" s="2" t="n">
         <v>2230</v>
@@ -3825,7 +3593,7 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>23</v>
+        <v>1023</v>
       </c>
       <c r="B95" s="2" t="n">
         <v>2231</v>
@@ -3845,7 +3613,7 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>24</v>
+        <v>1024</v>
       </c>
       <c r="B96" s="2" t="n">
         <v>2232</v>
@@ -3865,7 +3633,7 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>25</v>
+        <v>1025</v>
       </c>
       <c r="B97" s="2" t="n">
         <v>2233</v>
@@ -3885,7 +3653,7 @@
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>26</v>
+        <v>1026</v>
       </c>
       <c r="B98" s="2" t="n">
         <v>2234</v>
@@ -3905,7 +3673,7 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>27</v>
+        <v>1027</v>
       </c>
       <c r="B99" s="2" t="n">
         <v>2235</v>
@@ -3925,7 +3693,7 @@
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>28</v>
+        <v>1028</v>
       </c>
       <c r="B100" s="2" t="n">
         <v>2236</v>
@@ -3945,7 +3713,7 @@
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>29</v>
+        <v>1029</v>
       </c>
       <c r="B101" s="2" t="n">
         <v>2236</v>
@@ -3965,7 +3733,7 @@
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>30</v>
+        <v>1030</v>
       </c>
       <c r="B102" s="2" t="n">
         <v>2237</v>
@@ -3985,7 +3753,7 @@
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>31</v>
+        <v>1031</v>
       </c>
       <c r="B103" s="2" t="n">
         <v>2238</v>
@@ -4005,7 +3773,7 @@
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>32</v>
+        <v>1032</v>
       </c>
       <c r="B104" s="2" t="n">
         <v>2238</v>
@@ -4025,67 +3793,67 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>34</v>
+        <v>1033</v>
       </c>
       <c r="B105" s="2" t="n">
         <v>2239</v>
       </c>
       <c r="C105" s="2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D105" s="2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E105" s="2" t="n"/>
       <c r="F105" s="2" t="n">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="G105" s="2" t="n"/>
       <c r="H105" s="2" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>35</v>
+        <v>1034</v>
       </c>
       <c r="B106" s="2" t="n">
         <v>2239</v>
       </c>
       <c r="C106" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D106" s="2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E106" s="2" t="n"/>
       <c r="F106" s="2" t="n">
-        <v>490</v>
+        <v>100</v>
       </c>
       <c r="G106" s="2" t="n"/>
       <c r="H106" s="2" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>33</v>
+        <v>1035</v>
       </c>
       <c r="B107" s="2" t="n">
         <v>2239</v>
       </c>
       <c r="C107" s="2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D107" s="2" t="n">
         <v>7</v>
       </c>
       <c r="E107" s="2" t="n"/>
       <c r="F107" s="2" t="n">
-        <v>350</v>
+        <v>490</v>
       </c>
       <c r="G107" s="2" t="n"/>
       <c r="H107" s="2" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>36</v>
+        <v>1036</v>
       </c>
       <c r="B108" s="2" t="n">
         <v>2240</v>
@@ -4105,7 +3873,7 @@
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>37</v>
+        <v>1037</v>
       </c>
       <c r="B109" s="2" t="n">
         <v>2241</v>
@@ -4125,7 +3893,7 @@
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>38</v>
+        <v>1038</v>
       </c>
       <c r="B110" s="2" t="n">
         <v>2242</v>
@@ -4145,7 +3913,7 @@
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>39</v>
+        <v>1039</v>
       </c>
       <c r="B111" s="2" t="n">
         <v>2243</v>
@@ -4165,7 +3933,7 @@
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>40</v>
+        <v>1040</v>
       </c>
       <c r="B112" s="2" t="n">
         <v>2244</v>
@@ -4185,7 +3953,7 @@
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>41</v>
+        <v>1041</v>
       </c>
       <c r="B113" s="2" t="n">
         <v>2244</v>
@@ -4205,47 +3973,47 @@
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>43</v>
+        <v>1042</v>
       </c>
       <c r="B114" s="2" t="n">
         <v>2245</v>
       </c>
       <c r="C114" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D114" s="2" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E114" s="2" t="n"/>
       <c r="F114" s="2" t="n">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="G114" s="2" t="n"/>
       <c r="H114" s="2" t="n"/>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>42</v>
+        <v>1043</v>
       </c>
       <c r="B115" s="2" t="n">
         <v>2245</v>
       </c>
       <c r="C115" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D115" s="2" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E115" s="2" t="n"/>
       <c r="F115" s="2" t="n">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="G115" s="2" t="n"/>
       <c r="H115" s="2" t="n"/>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>44</v>
+        <v>1044</v>
       </c>
       <c r="B116" s="2" t="n">
         <v>2246</v>
@@ -4265,7 +4033,7 @@
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>45</v>
+        <v>1045</v>
       </c>
       <c r="B117" s="2" t="n">
         <v>2247</v>
@@ -4285,7 +4053,7 @@
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>46</v>
+        <v>1046</v>
       </c>
       <c r="B118" s="2" t="n">
         <v>2248</v>
@@ -4305,7 +4073,7 @@
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>47</v>
+        <v>1047</v>
       </c>
       <c r="B119" s="2" t="n">
         <v>2249</v>
@@ -4325,7 +4093,7 @@
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>48</v>
+        <v>1048</v>
       </c>
       <c r="B120" s="2" t="n">
         <v>2250</v>
@@ -4345,7 +4113,7 @@
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>49</v>
+        <v>1049</v>
       </c>
       <c r="B121" s="2" t="n">
         <v>2251</v>
@@ -4365,7 +4133,7 @@
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>50</v>
+        <v>1050</v>
       </c>
       <c r="B122" s="2" t="n">
         <v>2252</v>
@@ -4385,7 +4153,7 @@
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>51</v>
+        <v>1051</v>
       </c>
       <c r="B123" s="2" t="n">
         <v>2253</v>
@@ -4405,7 +4173,7 @@
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>52</v>
+        <v>1052</v>
       </c>
       <c r="B124" s="2" t="n">
         <v>2254</v>
@@ -4425,7 +4193,7 @@
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>53</v>
+        <v>1053</v>
       </c>
       <c r="B125" s="2" t="n">
         <v>2255</v>
@@ -4445,7 +4213,7 @@
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>54</v>
+        <v>1054</v>
       </c>
       <c r="B126" s="2" t="n">
         <v>2256</v>
@@ -4465,7 +4233,7 @@
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>55</v>
+        <v>1055</v>
       </c>
       <c r="B127" s="2" t="n">
         <v>2257</v>
@@ -4485,7 +4253,7 @@
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>56</v>
+        <v>1056</v>
       </c>
       <c r="B128" s="2" t="n">
         <v>2258</v>
@@ -4505,7 +4273,7 @@
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>57</v>
+        <v>1057</v>
       </c>
       <c r="B129" s="2" t="n">
         <v>2259</v>
@@ -4525,7 +4293,7 @@
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>58</v>
+        <v>1058</v>
       </c>
       <c r="B130" s="2" t="n">
         <v>2260</v>
@@ -4545,7 +4313,7 @@
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>59</v>
+        <v>1059</v>
       </c>
       <c r="B131" s="2" t="n">
         <v>2261</v>
@@ -4565,7 +4333,7 @@
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>60</v>
+        <v>1060</v>
       </c>
       <c r="B132" s="2" t="n">
         <v>2262</v>
@@ -4585,7 +4353,7 @@
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>61</v>
+        <v>1061</v>
       </c>
       <c r="B133" s="2" t="n">
         <v>2263</v>
@@ -4605,7 +4373,7 @@
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>62</v>
+        <v>1062</v>
       </c>
       <c r="B134" s="2" t="n">
         <v>2264</v>
@@ -4625,7 +4393,7 @@
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>63</v>
+        <v>1063</v>
       </c>
       <c r="B135" s="2" t="n">
         <v>2265</v>
@@ -4645,7 +4413,7 @@
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>64</v>
+        <v>1064</v>
       </c>
       <c r="B136" s="2" t="n">
         <v>2266</v>
@@ -4665,7 +4433,7 @@
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>65</v>
+        <v>1065</v>
       </c>
       <c r="B137" s="2" t="n">
         <v>2266</v>
@@ -4685,7 +4453,7 @@
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>66</v>
+        <v>1066</v>
       </c>
       <c r="B138" s="2" t="n">
         <v>2266</v>
@@ -4705,87 +4473,87 @@
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>69</v>
+        <v>1067</v>
       </c>
       <c r="B139" s="2" t="n">
         <v>2267</v>
       </c>
       <c r="C139" s="2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D139" s="2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E139" s="2" t="n"/>
       <c r="F139" s="2" t="n">
-        <v>40</v>
+        <v>450</v>
       </c>
       <c r="G139" s="2" t="n"/>
       <c r="H139" s="2" t="n"/>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>70</v>
+        <v>1068</v>
       </c>
       <c r="B140" s="2" t="n">
         <v>2267</v>
       </c>
       <c r="C140" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D140" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E140" s="2" t="n"/>
       <c r="F140" s="2" t="n">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="G140" s="2" t="n"/>
       <c r="H140" s="2" t="n"/>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>67</v>
+        <v>1069</v>
       </c>
       <c r="B141" s="2" t="n">
         <v>2267</v>
       </c>
       <c r="C141" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D141" s="2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E141" s="2" t="n"/>
       <c r="F141" s="2" t="n">
-        <v>450</v>
+        <v>40</v>
       </c>
       <c r="G141" s="2" t="n"/>
       <c r="H141" s="2" t="n"/>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>68</v>
+        <v>1070</v>
       </c>
       <c r="B142" s="2" t="n">
         <v>2267</v>
       </c>
       <c r="C142" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D142" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E142" s="2" t="n"/>
       <c r="F142" s="2" t="n">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="G142" s="2" t="n"/>
       <c r="H142" s="2" t="n"/>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>71</v>
+        <v>1071</v>
       </c>
       <c r="B143" s="2" t="n">
         <v>2267</v>

</xml_diff>